<commit_message>
corrected the error of pronoun calculation
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -537,25 +537,25 @@
         <v>27.96551724137931</v>
       </c>
       <c r="H2" t="n">
-        <v>67.07768187422934</v>
+        <v>60.17262638717632</v>
       </c>
       <c r="I2" t="n">
-        <v>11.45451762404864</v>
+        <v>11.42689740210043</v>
       </c>
       <c r="J2" t="n">
         <v>27.96551724137931</v>
       </c>
       <c r="K2" t="n">
-        <v>544</v>
+        <v>488</v>
       </c>
       <c r="L2" t="n">
         <v>811</v>
       </c>
       <c r="M2" t="n">
-        <v>3.683107274969174</v>
+        <v>3.316892725030826</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O2" t="n">
         <v>9.42170160295931</v>
@@ -588,25 +588,25 @@
         <v>18.10344827586207</v>
       </c>
       <c r="H3" t="n">
-        <v>61.90476190476191</v>
+        <v>54.47619047619048</v>
       </c>
       <c r="I3" t="n">
-        <v>7.488998357963876</v>
+        <v>7.45928407224959</v>
       </c>
       <c r="J3" t="n">
         <v>18.10344827586207</v>
       </c>
       <c r="K3" t="n">
-        <v>650</v>
+        <v>572</v>
       </c>
       <c r="L3" t="n">
         <v>1050</v>
       </c>
       <c r="M3" t="n">
-        <v>3.422857142857143</v>
+        <v>3.052380952380952</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="O3" t="n">
         <v>8.80952380952381</v>
@@ -639,25 +639,25 @@
         <v>23.1</v>
       </c>
       <c r="H4" t="n">
-        <v>63.41991341991342</v>
+        <v>56.92640692640693</v>
       </c>
       <c r="I4" t="n">
-        <v>9.493679653679655</v>
+        <v>9.467705627705628</v>
       </c>
       <c r="J4" t="n">
         <v>23.1</v>
       </c>
       <c r="K4" t="n">
-        <v>586</v>
+        <v>526</v>
       </c>
       <c r="L4" t="n">
         <v>924</v>
       </c>
       <c r="M4" t="n">
-        <v>3.494588744588745</v>
+        <v>3.154761904761905</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O4" t="n">
         <v>8.930735930735931</v>
@@ -690,25 +690,25 @@
         <v>22.91304347826087</v>
       </c>
       <c r="H5" t="n">
-        <v>68.59582542694497</v>
+        <v>59.01328273244781</v>
       </c>
       <c r="I5" t="n">
-        <v>9.43960069301213</v>
+        <v>9.401270522234141</v>
       </c>
       <c r="J5" t="n">
         <v>22.91304347826087</v>
       </c>
       <c r="K5" t="n">
-        <v>723</v>
+        <v>622</v>
       </c>
       <c r="L5" t="n">
         <v>1054</v>
       </c>
       <c r="M5" t="n">
-        <v>3.566413662239089</v>
+        <v>3.11100569259962</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O5" t="n">
         <v>9.193548387096774</v>
@@ -741,25 +741,25 @@
         <v>12.96116504854369</v>
       </c>
       <c r="H6" t="n">
-        <v>56.32958801498127</v>
+        <v>49.66292134831461</v>
       </c>
       <c r="I6" t="n">
-        <v>5.409784371477401</v>
+        <v>5.383117704810735</v>
       </c>
       <c r="J6" t="n">
         <v>12.96116504854369</v>
       </c>
       <c r="K6" t="n">
-        <v>752</v>
+        <v>663</v>
       </c>
       <c r="L6" t="n">
         <v>1335</v>
       </c>
       <c r="M6" t="n">
-        <v>3.210486891385768</v>
+        <v>2.893632958801498</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O6" t="n">
         <v>8.28689138576779</v>
@@ -792,25 +792,25 @@
         <v>27.96551724137931</v>
       </c>
       <c r="H7" t="n">
-        <v>67.07768187422934</v>
+        <v>60.17262638717632</v>
       </c>
       <c r="I7" t="n">
-        <v>11.45451762404864</v>
+        <v>11.42689740210043</v>
       </c>
       <c r="J7" t="n">
         <v>27.96551724137931</v>
       </c>
       <c r="K7" t="n">
-        <v>544</v>
+        <v>488</v>
       </c>
       <c r="L7" t="n">
         <v>811</v>
       </c>
       <c r="M7" t="n">
-        <v>3.683107274969174</v>
+        <v>3.316892725030826</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O7" t="n">
         <v>9.42170160295931</v>
@@ -843,25 +843,25 @@
         <v>18.10344827586207</v>
       </c>
       <c r="H8" t="n">
-        <v>61.90476190476191</v>
+        <v>54.47619047619048</v>
       </c>
       <c r="I8" t="n">
-        <v>7.488998357963876</v>
+        <v>7.45928407224959</v>
       </c>
       <c r="J8" t="n">
         <v>18.10344827586207</v>
       </c>
       <c r="K8" t="n">
-        <v>650</v>
+        <v>572</v>
       </c>
       <c r="L8" t="n">
         <v>1050</v>
       </c>
       <c r="M8" t="n">
-        <v>3.422857142857143</v>
+        <v>3.052380952380952</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="O8" t="n">
         <v>8.80952380952381</v>
@@ -894,25 +894,25 @@
         <v>23.1</v>
       </c>
       <c r="H9" t="n">
-        <v>63.41991341991342</v>
+        <v>56.92640692640693</v>
       </c>
       <c r="I9" t="n">
-        <v>9.493679653679655</v>
+        <v>9.467705627705628</v>
       </c>
       <c r="J9" t="n">
         <v>23.1</v>
       </c>
       <c r="K9" t="n">
-        <v>586</v>
+        <v>526</v>
       </c>
       <c r="L9" t="n">
         <v>924</v>
       </c>
       <c r="M9" t="n">
-        <v>3.494588744588745</v>
+        <v>3.154761904761905</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O9" t="n">
         <v>8.930735930735931</v>
@@ -945,25 +945,25 @@
         <v>22.91304347826087</v>
       </c>
       <c r="H10" t="n">
-        <v>68.59582542694497</v>
+        <v>59.01328273244781</v>
       </c>
       <c r="I10" t="n">
-        <v>9.43960069301213</v>
+        <v>9.401270522234141</v>
       </c>
       <c r="J10" t="n">
         <v>22.91304347826087</v>
       </c>
       <c r="K10" t="n">
-        <v>723</v>
+        <v>622</v>
       </c>
       <c r="L10" t="n">
         <v>1054</v>
       </c>
       <c r="M10" t="n">
-        <v>3.566413662239089</v>
+        <v>3.11100569259962</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O10" t="n">
         <v>9.193548387096774</v>
@@ -996,25 +996,25 @@
         <v>14.192</v>
       </c>
       <c r="H11" t="n">
-        <v>65.05073280721533</v>
+        <v>55.91882750845547</v>
       </c>
       <c r="I11" t="n">
-        <v>5.937002931228862</v>
+        <v>5.900475310033823</v>
       </c>
       <c r="J11" t="n">
         <v>14.192</v>
       </c>
       <c r="K11" t="n">
-        <v>1154</v>
+        <v>992</v>
       </c>
       <c r="L11" t="n">
         <v>1774</v>
       </c>
       <c r="M11" t="n">
-        <v>3.337655016910936</v>
+        <v>2.950394588500564</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O11" t="n">
         <v>8.455467869222097</v>
@@ -1047,25 +1047,25 @@
         <v>22.72093023255814</v>
       </c>
       <c r="H12" t="n">
-        <v>68.57727737973389</v>
+        <v>61.31013306038895</v>
       </c>
       <c r="I12" t="n">
-        <v>9.362681202542191</v>
+        <v>9.333612625264811</v>
       </c>
       <c r="J12" t="n">
         <v>22.72093023255814</v>
       </c>
       <c r="K12" t="n">
-        <v>670</v>
+        <v>599</v>
       </c>
       <c r="L12" t="n">
         <v>977</v>
       </c>
       <c r="M12" t="n">
-        <v>3.632548618219038</v>
+        <v>3.272262026612078</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O12" t="n">
         <v>9.221084953940634</v>
@@ -1098,25 +1098,25 @@
         <v>23.74468085106383</v>
       </c>
       <c r="H13" t="n">
-        <v>67.20430107526882</v>
+        <v>60.0358422939068</v>
       </c>
       <c r="I13" t="n">
-        <v>9.766689544726608</v>
+        <v>9.738015709601159</v>
       </c>
       <c r="J13" t="n">
         <v>23.74468085106383</v>
       </c>
       <c r="K13" t="n">
-        <v>750</v>
+        <v>670</v>
       </c>
       <c r="L13" t="n">
         <v>1116</v>
       </c>
       <c r="M13" t="n">
-        <v>3.531362007168459</v>
+        <v>3.181899641577061</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="O13" t="n">
         <v>9.049283154121865</v>
@@ -1149,25 +1149,25 @@
         <v>22.27906976744186</v>
       </c>
       <c r="H14" t="n">
-        <v>66.59707724425887</v>
+        <v>57.72442588726514</v>
       </c>
       <c r="I14" t="n">
-        <v>9.178016215953781</v>
+        <v>9.142525610525805</v>
       </c>
       <c r="J14" t="n">
         <v>22.27906976744186</v>
       </c>
       <c r="K14" t="n">
-        <v>638</v>
+        <v>553</v>
       </c>
       <c r="L14" t="n">
         <v>958</v>
       </c>
       <c r="M14" t="n">
-        <v>3.599164926931107</v>
+        <v>3.168058455114823</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="O14" t="n">
         <v>9.267223382045929</v>
@@ -1200,25 +1200,25 @@
         <v>24.28205128205128</v>
       </c>
       <c r="H15" t="n">
-        <v>68.6378035902851</v>
+        <v>60.19007391763463</v>
       </c>
       <c r="I15" t="n">
-        <v>9.987371727181653</v>
+        <v>9.953580808491052</v>
       </c>
       <c r="J15" t="n">
         <v>24.28205128205128</v>
       </c>
       <c r="K15" t="n">
-        <v>650</v>
+        <v>570</v>
       </c>
       <c r="L15" t="n">
         <v>947</v>
       </c>
       <c r="M15" t="n">
-        <v>3.664202745512144</v>
+        <v>3.251319957761352</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="O15" t="n">
         <v>9.327349524815206</v>
@@ -1251,25 +1251,25 @@
         <v>17.05747126436782</v>
       </c>
       <c r="H16" t="n">
-        <v>62.6010781671159</v>
+        <v>55.45822102425875</v>
       </c>
       <c r="I16" t="n">
-        <v>7.073392818415591</v>
+        <v>7.044821389844161</v>
       </c>
       <c r="J16" t="n">
         <v>17.05747126436782</v>
       </c>
       <c r="K16" t="n">
-        <v>929</v>
+        <v>823</v>
       </c>
       <c r="L16" t="n">
         <v>1484</v>
       </c>
       <c r="M16" t="n">
-        <v>3.331536388140162</v>
+        <v>2.962938005390836</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="O16" t="n">
         <v>8.661725067385445</v>
@@ -1302,25 +1302,25 @@
         <v>11.1484375</v>
       </c>
       <c r="H17" t="n">
-        <v>61.80798878766643</v>
+        <v>53.39873861247371</v>
       </c>
       <c r="I17" t="n">
-        <v>4.706606955150666</v>
+        <v>4.672969954449895</v>
       </c>
       <c r="J17" t="n">
         <v>11.1484375</v>
       </c>
       <c r="K17" t="n">
-        <v>882</v>
+        <v>762</v>
       </c>
       <c r="L17" t="n">
         <v>1427</v>
       </c>
       <c r="M17" t="n">
-        <v>3.292221443587947</v>
+        <v>2.871058163980378</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O17" t="n">
         <v>8.393833216538193</v>
@@ -1353,25 +1353,25 @@
         <v>19.11764705882353</v>
       </c>
       <c r="H18" t="n">
-        <v>65.84615384615384</v>
+        <v>56.12307692307692</v>
       </c>
       <c r="I18" t="n">
-        <v>7.910443438914027</v>
+        <v>7.871551131221719</v>
       </c>
       <c r="J18" t="n">
         <v>19.11764705882353</v>
       </c>
       <c r="K18" t="n">
-        <v>1070</v>
+        <v>912</v>
       </c>
       <c r="L18" t="n">
         <v>1625</v>
       </c>
       <c r="M18" t="n">
-        <v>3.433230769230769</v>
+        <v>3.004923076923077</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="O18" t="n">
         <v>8.764923076923077</v>
@@ -1404,25 +1404,25 @@
         <v>21.86842105263158</v>
       </c>
       <c r="H19" t="n">
-        <v>66.66666666666666</v>
+        <v>59.08543922984356</v>
       </c>
       <c r="I19" t="n">
-        <v>9.014035087719298</v>
+        <v>8.983710177972005</v>
       </c>
       <c r="J19" t="n">
         <v>21.86842105263158</v>
       </c>
       <c r="K19" t="n">
-        <v>554</v>
+        <v>491</v>
       </c>
       <c r="L19" t="n">
         <v>831</v>
       </c>
       <c r="M19" t="n">
-        <v>3.690734055354994</v>
+        <v>3.287605294825511</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O19" t="n">
         <v>9.393501805054152</v>
@@ -1455,25 +1455,25 @@
         <v>14.95</v>
       </c>
       <c r="H20" t="n">
-        <v>60.53511705685619</v>
+        <v>51.50501672240802</v>
       </c>
       <c r="I20" t="n">
-        <v>6.222140468227425</v>
+        <v>6.186020066889633</v>
       </c>
       <c r="J20" t="n">
         <v>14.95</v>
       </c>
       <c r="K20" t="n">
-        <v>905</v>
+        <v>770</v>
       </c>
       <c r="L20" t="n">
         <v>1495</v>
       </c>
       <c r="M20" t="n">
-        <v>3.357859531772575</v>
+        <v>2.912374581939799</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O20" t="n">
         <v>8.549832775919732</v>
@@ -1506,25 +1506,25 @@
         <v>18.03448275862069</v>
       </c>
       <c r="H21" t="n">
-        <v>64.43594646271511</v>
+        <v>54.97131931166348</v>
       </c>
       <c r="I21" t="n">
-        <v>7.471536889299137</v>
+        <v>7.43367838069493</v>
       </c>
       <c r="J21" t="n">
         <v>18.03448275862069</v>
       </c>
       <c r="K21" t="n">
-        <v>674</v>
+        <v>575</v>
       </c>
       <c r="L21" t="n">
         <v>1046</v>
       </c>
       <c r="M21" t="n">
-        <v>3.509560229445507</v>
+        <v>3.073613766730401</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O21" t="n">
         <v>8.921606118546846</v>
@@ -1557,25 +1557,25 @@
         <v>20.24390243902439</v>
       </c>
       <c r="H22" t="n">
-        <v>66.98795180722892</v>
+        <v>58.19277108433734</v>
       </c>
       <c r="I22" t="n">
-        <v>8.365512782838671</v>
+        <v>8.330332059947105</v>
       </c>
       <c r="J22" t="n">
         <v>20.24390243902439</v>
       </c>
       <c r="K22" t="n">
-        <v>556</v>
+        <v>483</v>
       </c>
       <c r="L22" t="n">
         <v>830</v>
       </c>
       <c r="M22" t="n">
-        <v>3.687951807228916</v>
+        <v>3.259036144578313</v>
       </c>
       <c r="N22" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O22" t="n">
         <v>9.349397590361447</v>
@@ -1608,25 +1608,25 @@
         <v>20.75609756097561</v>
       </c>
       <c r="H23" t="n">
-        <v>68.86016451233843</v>
+        <v>61.33960047003525</v>
       </c>
       <c r="I23" t="n">
-        <v>8.577879682439599</v>
+        <v>8.547797426270385</v>
       </c>
       <c r="J23" t="n">
         <v>20.75609756097561</v>
       </c>
       <c r="K23" t="n">
-        <v>586</v>
+        <v>522</v>
       </c>
       <c r="L23" t="n">
         <v>851</v>
       </c>
       <c r="M23" t="n">
-        <v>3.722679200940071</v>
+        <v>3.347826086956522</v>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O23" t="n">
         <v>9.471210340775558</v>
@@ -1659,25 +1659,25 @@
         <v>21.05</v>
       </c>
       <c r="H24" t="n">
-        <v>67.3396674584323</v>
+        <v>59.14489311163895</v>
       </c>
       <c r="I24" t="n">
-        <v>8.68935866983373</v>
+        <v>8.656579572446557</v>
       </c>
       <c r="J24" t="n">
         <v>21.05</v>
       </c>
       <c r="K24" t="n">
-        <v>567</v>
+        <v>498</v>
       </c>
       <c r="L24" t="n">
         <v>842</v>
       </c>
       <c r="M24" t="n">
-        <v>3.675771971496437</v>
+        <v>3.276722090261283</v>
       </c>
       <c r="N24" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O24" t="n">
         <v>9.396674584323041</v>
@@ -1710,25 +1710,25 @@
         <v>20.51219512195122</v>
       </c>
       <c r="H25" t="n">
-        <v>70.27348394768134</v>
+        <v>61.23662306777645</v>
       </c>
       <c r="I25" t="n">
-        <v>8.485971984571213</v>
+        <v>8.449824541051594</v>
       </c>
       <c r="J25" t="n">
         <v>20.51219512195122</v>
       </c>
       <c r="K25" t="n">
-        <v>591</v>
+        <v>515</v>
       </c>
       <c r="L25" t="n">
         <v>841</v>
       </c>
       <c r="M25" t="n">
-        <v>3.763376932223543</v>
+        <v>3.33769322235434</v>
       </c>
       <c r="N25" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O25" t="n">
         <v>9.510107015457788</v>
@@ -1761,25 +1761,25 @@
         <v>20.68292682926829</v>
       </c>
       <c r="H26" t="n">
-        <v>69.5754716981132</v>
+        <v>61.43867924528303</v>
       </c>
       <c r="I26" t="n">
-        <v>8.551472618499771</v>
+        <v>8.518925448688449</v>
       </c>
       <c r="J26" t="n">
         <v>20.68292682926829</v>
       </c>
       <c r="K26" t="n">
-        <v>590</v>
+        <v>521</v>
       </c>
       <c r="L26" t="n">
         <v>848</v>
       </c>
       <c r="M26" t="n">
-        <v>3.725235849056604</v>
+        <v>3.326650943396226</v>
       </c>
       <c r="N26" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O26" t="n">
         <v>9.464622641509434</v>
@@ -1812,25 +1812,25 @@
         <v>19.63636363636364</v>
       </c>
       <c r="H27" t="n">
-        <v>68.05555555555556</v>
+        <v>59.49074074074075</v>
       </c>
       <c r="I27" t="n">
-        <v>8.126767676767678</v>
+        <v>8.092508417508418</v>
       </c>
       <c r="J27" t="n">
         <v>19.63636363636364</v>
       </c>
       <c r="K27" t="n">
-        <v>588</v>
+        <v>514</v>
       </c>
       <c r="L27" t="n">
         <v>864</v>
       </c>
       <c r="M27" t="n">
-        <v>3.666666666666667</v>
+        <v>3.251157407407407</v>
       </c>
       <c r="N27" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O27" t="n">
         <v>9.32175925925926</v>
@@ -1863,25 +1863,25 @@
         <v>18.81666666666667</v>
       </c>
       <c r="H28" t="n">
-        <v>59.96457041629761</v>
+        <v>51.90434012400355</v>
       </c>
       <c r="I28" t="n">
-        <v>7.766524948331858</v>
+        <v>7.734284027162682</v>
       </c>
       <c r="J28" t="n">
         <v>18.81666666666667</v>
       </c>
       <c r="K28" t="n">
-        <v>677</v>
+        <v>586</v>
       </c>
       <c r="L28" t="n">
         <v>1129</v>
       </c>
       <c r="M28" t="n">
-        <v>3.331266607617361</v>
+        <v>2.953055801594331</v>
       </c>
       <c r="N28" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O28" t="n">
         <v>8.705048715677592</v>
@@ -1914,25 +1914,25 @@
         <v>20.58928571428572</v>
       </c>
       <c r="H29" t="n">
-        <v>62.70598438855161</v>
+        <v>54.81352992194276</v>
       </c>
       <c r="I29" t="n">
-        <v>8.486538223268493</v>
+        <v>8.454968405402058</v>
       </c>
       <c r="J29" t="n">
         <v>20.58928571428572</v>
       </c>
       <c r="K29" t="n">
-        <v>723</v>
+        <v>632</v>
       </c>
       <c r="L29" t="n">
         <v>1153</v>
       </c>
       <c r="M29" t="n">
-        <v>3.367736339982654</v>
+        <v>2.998265394622723</v>
       </c>
       <c r="N29" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O29" t="n">
         <v>8.722463139635733</v>
@@ -1965,25 +1965,25 @@
         <v>17.55384615384616</v>
       </c>
       <c r="H30" t="n">
-        <v>63.27782646801051</v>
+        <v>53.54951796669588</v>
       </c>
       <c r="I30" t="n">
-        <v>7.274649767410505</v>
+        <v>7.235736533405246</v>
       </c>
       <c r="J30" t="n">
         <v>17.55384615384616</v>
       </c>
       <c r="K30" t="n">
-        <v>722</v>
+        <v>611</v>
       </c>
       <c r="L30" t="n">
         <v>1141</v>
       </c>
       <c r="M30" t="n">
-        <v>3.418054338299737</v>
+        <v>2.983347940403155</v>
       </c>
       <c r="N30" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="O30" t="n">
         <v>8.860648553900088</v>
@@ -2016,25 +2016,25 @@
         <v>18.14285714285714</v>
       </c>
       <c r="H31" t="n">
-        <v>66.05424321959755</v>
+        <v>56.86789151356081</v>
       </c>
       <c r="I31" t="n">
-        <v>7.521359830021247</v>
+        <v>7.4846144231971</v>
       </c>
       <c r="J31" t="n">
         <v>18.14285714285714</v>
       </c>
       <c r="K31" t="n">
-        <v>755</v>
+        <v>650</v>
       </c>
       <c r="L31" t="n">
         <v>1143</v>
       </c>
       <c r="M31" t="n">
-        <v>3.470691163604549</v>
+        <v>3.063867016622922</v>
       </c>
       <c r="N31" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O31" t="n">
         <v>8.797025371828521</v>
@@ -2067,25 +2067,25 @@
         <v>16.93548387096774</v>
       </c>
       <c r="H32" t="n">
-        <v>65.14285714285715</v>
+        <v>57.52380952380952</v>
       </c>
       <c r="I32" t="n">
-        <v>7.034764976958525</v>
+        <v>7.004288786482334</v>
       </c>
       <c r="J32" t="n">
         <v>16.93548387096774</v>
       </c>
       <c r="K32" t="n">
-        <v>684</v>
+        <v>604</v>
       </c>
       <c r="L32" t="n">
         <v>1050</v>
       </c>
       <c r="M32" t="n">
-        <v>3.495238095238095</v>
+        <v>3.12952380952381</v>
       </c>
       <c r="N32" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O32" t="n">
         <v>8.98952380952381</v>
@@ -2118,25 +2118,25 @@
         <v>22.34545454545454</v>
       </c>
       <c r="H33" t="n">
-        <v>64.19853539462979</v>
+        <v>54.8413344182262</v>
       </c>
       <c r="I33" t="n">
-        <v>9.194975959760336</v>
+        <v>9.157547155854722</v>
       </c>
       <c r="J33" t="n">
         <v>22.34545454545454</v>
       </c>
       <c r="K33" t="n">
-        <v>789</v>
+        <v>674</v>
       </c>
       <c r="L33" t="n">
         <v>1229</v>
       </c>
       <c r="M33" t="n">
-        <v>3.484947111472742</v>
+        <v>3.054515866558178</v>
       </c>
       <c r="N33" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="O33" t="n">
         <v>8.938161106590725</v>
@@ -2169,25 +2169,25 @@
         <v>16.59340659340659</v>
       </c>
       <c r="H34" t="n">
-        <v>61.65562913907284</v>
+        <v>52.71523178807948</v>
       </c>
       <c r="I34" t="n">
-        <v>6.88398515391893</v>
+        <v>6.848223564514957</v>
       </c>
       <c r="J34" t="n">
         <v>16.59340659340659</v>
       </c>
       <c r="K34" t="n">
-        <v>931</v>
+        <v>796</v>
       </c>
       <c r="L34" t="n">
         <v>1510</v>
       </c>
       <c r="M34" t="n">
-        <v>3.312582781456954</v>
+        <v>2.917880794701987</v>
       </c>
       <c r="N34" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O34" t="n">
         <v>8.479470198675497</v>
@@ -2220,25 +2220,25 @@
         <v>20.36734693877551</v>
       </c>
       <c r="H35" t="n">
-        <v>64.52905811623246</v>
+        <v>56.1122244488978</v>
       </c>
       <c r="I35" t="n">
-        <v>8.405055007975134</v>
+        <v>8.371387673305795</v>
       </c>
       <c r="J35" t="n">
         <v>20.36734693877551</v>
       </c>
       <c r="K35" t="n">
-        <v>644</v>
+        <v>560</v>
       </c>
       <c r="L35" t="n">
         <v>998</v>
       </c>
       <c r="M35" t="n">
-        <v>3.466933867735471</v>
+        <v>3.074148296593187</v>
       </c>
       <c r="N35" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O35" t="n">
         <v>8.965931863727455</v>
@@ -2271,25 +2271,25 @@
         <v>11.10126582278481</v>
       </c>
       <c r="H36" t="n">
-        <v>56.61345496009123</v>
+        <v>49.03078677309008</v>
       </c>
       <c r="I36" t="n">
-        <v>4.666960148954289</v>
+        <v>4.636629476206284</v>
       </c>
       <c r="J36" t="n">
         <v>11.10126582278481</v>
       </c>
       <c r="K36" t="n">
-        <v>993</v>
+        <v>860</v>
       </c>
       <c r="L36" t="n">
         <v>1754</v>
       </c>
       <c r="M36" t="n">
-        <v>3.129988597491448</v>
+        <v>2.787913340935006</v>
       </c>
       <c r="N36" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O36" t="n">
         <v>8.254846066134549</v>
@@ -2322,25 +2322,25 @@
         <v>13.59139784946237</v>
       </c>
       <c r="H37" t="n">
-        <v>61.62974683544304</v>
+        <v>53.63924050632911</v>
       </c>
       <c r="I37" t="n">
-        <v>5.683078127126719</v>
+        <v>5.651116101810263</v>
       </c>
       <c r="J37" t="n">
         <v>13.59139784946237</v>
       </c>
       <c r="K37" t="n">
-        <v>779</v>
+        <v>678</v>
       </c>
       <c r="L37" t="n">
         <v>1264</v>
       </c>
       <c r="M37" t="n">
-        <v>3.380537974683544</v>
+        <v>2.988924050632912</v>
       </c>
       <c r="N37" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O37" t="n">
         <v>8.666139240506329</v>
@@ -2373,25 +2373,25 @@
         <v>14.93827160493827</v>
       </c>
       <c r="H38" t="n">
-        <v>67.60330578512396</v>
+        <v>59.42148760330579</v>
       </c>
       <c r="I38" t="n">
-        <v>6.245721865115804</v>
+        <v>6.212994592388533</v>
       </c>
       <c r="J38" t="n">
         <v>14.93827160493827</v>
       </c>
       <c r="K38" t="n">
-        <v>818</v>
+        <v>719</v>
       </c>
       <c r="L38" t="n">
         <v>1210</v>
       </c>
       <c r="M38" t="n">
-        <v>3.533884297520661</v>
+        <v>3.150413223140496</v>
       </c>
       <c r="N38" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="O38" t="n">
         <v>8.99504132231405</v>
@@ -2424,25 +2424,25 @@
         <v>18.67123287671233</v>
       </c>
       <c r="H39" t="n">
-        <v>64.19662509170946</v>
+        <v>56.71313279530447</v>
       </c>
       <c r="I39" t="n">
-        <v>7.725279651051769</v>
+        <v>7.69534568186615</v>
       </c>
       <c r="J39" t="n">
         <v>18.67123287671233</v>
       </c>
       <c r="K39" t="n">
-        <v>875</v>
+        <v>773</v>
       </c>
       <c r="L39" t="n">
         <v>1363</v>
       </c>
       <c r="M39" t="n">
-        <v>3.407923697725605</v>
+        <v>3.047688921496698</v>
       </c>
       <c r="N39" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O39" t="n">
         <v>8.694057226705796</v>
@@ -2475,25 +2475,25 @@
         <v>11.68148148148148</v>
       </c>
       <c r="H40" t="n">
-        <v>57.32403297400127</v>
+        <v>50.34876347495244</v>
       </c>
       <c r="I40" t="n">
-        <v>4.901888724488598</v>
+        <v>4.873987646492402</v>
       </c>
       <c r="J40" t="n">
         <v>11.68148148148148</v>
       </c>
       <c r="K40" t="n">
-        <v>904</v>
+        <v>794</v>
       </c>
       <c r="L40" t="n">
         <v>1577</v>
       </c>
       <c r="M40" t="n">
-        <v>3.159797083069118</v>
+        <v>2.840202916930882</v>
       </c>
       <c r="N40" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="O40" t="n">
         <v>8.098287888395689</v>
@@ -2526,25 +2526,25 @@
         <v>11.72340425531915</v>
       </c>
       <c r="H41" t="n">
-        <v>57.62250453720507</v>
+        <v>51.17967332123412</v>
       </c>
       <c r="I41" t="n">
-        <v>4.91985172027648</v>
+        <v>4.894080395412597</v>
       </c>
       <c r="J41" t="n">
         <v>11.72340425531915</v>
       </c>
       <c r="K41" t="n">
-        <v>635</v>
+        <v>564</v>
       </c>
       <c r="L41" t="n">
         <v>1102</v>
       </c>
       <c r="M41" t="n">
-        <v>3.323049001814882</v>
+        <v>2.990018148820327</v>
       </c>
       <c r="N41" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O41" t="n">
         <v>8.526315789473685</v>
@@ -2577,25 +2577,25 @@
         <v>28.37142857142857</v>
       </c>
       <c r="H42" t="n">
-        <v>63.94763343403827</v>
+        <v>57.30110775427995</v>
       </c>
       <c r="I42" t="n">
-        <v>11.60436196230758</v>
+        <v>11.57777585958855</v>
       </c>
       <c r="J42" t="n">
         <v>28.37142857142857</v>
       </c>
       <c r="K42" t="n">
-        <v>635</v>
+        <v>569</v>
       </c>
       <c r="L42" t="n">
         <v>993</v>
       </c>
       <c r="M42" t="n">
-        <v>3.531722054380665</v>
+        <v>3.171198388721047</v>
       </c>
       <c r="N42" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O42" t="n">
         <v>9.021148036253777</v>
@@ -2628,25 +2628,25 @@
         <v>24.6969696969697</v>
       </c>
       <c r="H43" t="n">
-        <v>66.13496932515336</v>
+        <v>59.2638036809816</v>
       </c>
       <c r="I43" t="n">
-        <v>10.14332775608849</v>
+        <v>10.11584309351181</v>
       </c>
       <c r="J43" t="n">
         <v>24.6969696969697</v>
       </c>
       <c r="K43" t="n">
-        <v>539</v>
+        <v>483</v>
       </c>
       <c r="L43" t="n">
         <v>815</v>
       </c>
       <c r="M43" t="n">
-        <v>3.656441717791411</v>
+        <v>3.296932515337423</v>
       </c>
       <c r="N43" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="O43" t="n">
         <v>9.267484662576686</v>
@@ -2679,25 +2679,25 @@
         <v>19.15555555555556</v>
       </c>
       <c r="H44" t="n">
-        <v>66.70533642691416</v>
+        <v>59.86078886310905</v>
       </c>
       <c r="I44" t="n">
-        <v>7.929043567929878</v>
+        <v>7.901665377674658</v>
       </c>
       <c r="J44" t="n">
         <v>19.15555555555556</v>
       </c>
       <c r="K44" t="n">
-        <v>575</v>
+        <v>516</v>
       </c>
       <c r="L44" t="n">
         <v>862</v>
       </c>
       <c r="M44" t="n">
-        <v>3.610208816705336</v>
+        <v>3.265661252900232</v>
       </c>
       <c r="N44" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="O44" t="n">
         <v>9.196055684454757</v>
@@ -2730,25 +2730,25 @@
         <v>20.5</v>
       </c>
       <c r="H45" t="n">
-        <v>65</v>
+        <v>58.78048780487804</v>
       </c>
       <c r="I45" t="n">
-        <v>8.459999999999999</v>
+        <v>8.435121951219513</v>
       </c>
       <c r="J45" t="n">
         <v>20.5</v>
       </c>
       <c r="K45" t="n">
-        <v>533</v>
+        <v>482</v>
       </c>
       <c r="L45" t="n">
         <v>820</v>
       </c>
       <c r="M45" t="n">
-        <v>3.615853658536585</v>
+        <v>3.276829268292683</v>
       </c>
       <c r="N45" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="O45" t="n">
         <v>9.223170731707317</v>
@@ -2781,25 +2781,25 @@
         <v>14.18333333333333</v>
       </c>
       <c r="H46" t="n">
-        <v>65.33490011750881</v>
+        <v>58.75440658049354</v>
       </c>
       <c r="I46" t="n">
-        <v>5.93467293380337</v>
+        <v>5.908350959655309</v>
       </c>
       <c r="J46" t="n">
         <v>14.18333333333333</v>
       </c>
       <c r="K46" t="n">
-        <v>556</v>
+        <v>500</v>
       </c>
       <c r="L46" t="n">
         <v>851</v>
       </c>
       <c r="M46" t="n">
-        <v>3.562867215041128</v>
+        <v>3.220916568742656</v>
       </c>
       <c r="N46" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="O46" t="n">
         <v>9.142185663924794</v>
@@ -2832,25 +2832,25 @@
         <v>15.55128205128205</v>
       </c>
       <c r="H47" t="n">
-        <v>60.42868920032976</v>
+        <v>50.20610057708161</v>
       </c>
       <c r="I47" t="n">
-        <v>6.46222757731414</v>
+        <v>6.421337222821148</v>
       </c>
       <c r="J47" t="n">
         <v>15.55128205128205</v>
       </c>
       <c r="K47" t="n">
-        <v>733</v>
+        <v>609</v>
       </c>
       <c r="L47" t="n">
         <v>1213</v>
       </c>
       <c r="M47" t="n">
-        <v>3.315746084089036</v>
+        <v>2.845836768342951</v>
       </c>
       <c r="N47" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="O47" t="n">
         <v>8.539983511953833</v>
@@ -2883,25 +2883,25 @@
         <v>28.53125</v>
       </c>
       <c r="H48" t="n">
-        <v>66.37458926615552</v>
+        <v>58.15991237677984</v>
       </c>
       <c r="I48" t="n">
-        <v>11.67799835706462</v>
+        <v>11.64513964950712</v>
       </c>
       <c r="J48" t="n">
         <v>28.53125</v>
       </c>
       <c r="K48" t="n">
-        <v>606</v>
+        <v>531</v>
       </c>
       <c r="L48" t="n">
         <v>913</v>
       </c>
       <c r="M48" t="n">
-        <v>3.559693318729463</v>
+        <v>3.153340635268346</v>
       </c>
       <c r="N48" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O48" t="n">
         <v>9.056955093099672</v>
@@ -2934,25 +2934,25 @@
         <v>35.07692307692308</v>
       </c>
       <c r="H49" t="n">
-        <v>65.78947368421053</v>
+        <v>58.11403508771929</v>
       </c>
       <c r="I49" t="n">
-        <v>14.29392712550607</v>
+        <v>14.26322537112011</v>
       </c>
       <c r="J49" t="n">
         <v>35.07692307692308</v>
       </c>
       <c r="K49" t="n">
-        <v>600</v>
+        <v>530</v>
       </c>
       <c r="L49" t="n">
         <v>912</v>
       </c>
       <c r="M49" t="n">
-        <v>3.554824561403509</v>
+        <v>3.161184210526316</v>
       </c>
       <c r="N49" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O49" t="n">
         <v>9.083333333333334</v>
@@ -2985,25 +2985,25 @@
         <v>31.14814814814815</v>
       </c>
       <c r="H50" t="n">
-        <v>64.56599286563615</v>
+        <v>57.90725326991677</v>
       </c>
       <c r="I50" t="n">
-        <v>12.7175232307218</v>
+        <v>12.69088827233893</v>
       </c>
       <c r="J50" t="n">
         <v>31.14814814814815</v>
       </c>
       <c r="K50" t="n">
-        <v>543</v>
+        <v>487</v>
       </c>
       <c r="L50" t="n">
         <v>841</v>
       </c>
       <c r="M50" t="n">
-        <v>3.604042806183115</v>
+        <v>3.253269916765755</v>
       </c>
       <c r="N50" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O50" t="n">
         <v>9.260404280618312</v>
@@ -3036,25 +3036,25 @@
         <v>33.4</v>
       </c>
       <c r="H51" t="n">
-        <v>66.34730538922156</v>
+        <v>59.52095808383233</v>
       </c>
       <c r="I51" t="n">
-        <v>13.62538922155689</v>
+        <v>13.59808383233533</v>
       </c>
       <c r="J51" t="n">
         <v>33.4</v>
       </c>
       <c r="K51" t="n">
-        <v>554</v>
+        <v>497</v>
       </c>
       <c r="L51" t="n">
         <v>835</v>
       </c>
       <c r="M51" t="n">
-        <v>3.658682634730539</v>
+        <v>3.280239520958084</v>
       </c>
       <c r="N51" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O51" t="n">
         <v>9.295808383233533</v>
@@ -3087,25 +3087,25 @@
         <v>21.27659574468085</v>
       </c>
       <c r="H52" t="n">
-        <v>63.1</v>
+        <v>52.7</v>
       </c>
       <c r="I52" t="n">
-        <v>8.76303829787234</v>
+        <v>8.721438297872341</v>
       </c>
       <c r="J52" t="n">
         <v>21.27659574468085</v>
       </c>
       <c r="K52" t="n">
-        <v>631</v>
+        <v>527</v>
       </c>
       <c r="L52" t="n">
         <v>1000</v>
       </c>
       <c r="M52" t="n">
-        <v>3.44</v>
+        <v>2.976</v>
       </c>
       <c r="N52" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="O52" t="n">
         <v>8.882999999999999</v>
@@ -3138,25 +3138,25 @@
         <v>24</v>
       </c>
       <c r="H53" t="n">
-        <v>61.51315789473685</v>
+        <v>55.26315789473685</v>
       </c>
       <c r="I53" t="n">
-        <v>9.846052631578949</v>
+        <v>9.821052631578949</v>
       </c>
       <c r="J53" t="n">
         <v>24</v>
       </c>
       <c r="K53" t="n">
-        <v>561</v>
+        <v>504</v>
       </c>
       <c r="L53" t="n">
         <v>912</v>
       </c>
       <c r="M53" t="n">
-        <v>3.490131578947369</v>
+        <v>3.145833333333333</v>
       </c>
       <c r="N53" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="O53" t="n">
         <v>8.949561403508772</v>
@@ -3189,25 +3189,25 @@
         <v>19.60869565217391</v>
       </c>
       <c r="H54" t="n">
-        <v>62.97117516629712</v>
+        <v>55.54323725055432</v>
       </c>
       <c r="I54" t="n">
-        <v>8.095362961534754</v>
+        <v>8.065651209871783</v>
       </c>
       <c r="J54" t="n">
         <v>19.60869565217391</v>
       </c>
       <c r="K54" t="n">
-        <v>568</v>
+        <v>501</v>
       </c>
       <c r="L54" t="n">
         <v>902</v>
       </c>
       <c r="M54" t="n">
-        <v>3.521064301552106</v>
+        <v>3.149667405764967</v>
       </c>
       <c r="N54" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="O54" t="n">
         <v>8.991130820399112</v>
@@ -3240,25 +3240,25 @@
         <v>19.40909090909091</v>
       </c>
       <c r="H55" t="n">
-        <v>66.86182669789227</v>
+        <v>60.4215456674473</v>
       </c>
       <c r="I55" t="n">
-        <v>8.031083670427932</v>
+        <v>8.005322546306154</v>
       </c>
       <c r="J55" t="n">
         <v>19.40909090909091</v>
       </c>
       <c r="K55" t="n">
-        <v>571</v>
+        <v>516</v>
       </c>
       <c r="L55" t="n">
         <v>854</v>
       </c>
       <c r="M55" t="n">
-        <v>3.640515222482436</v>
+        <v>3.2903981264637</v>
       </c>
       <c r="N55" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="O55" t="n">
         <v>9.270491803278688</v>
@@ -3291,25 +3291,25 @@
         <v>29.72413793103448</v>
       </c>
       <c r="H56" t="n">
-        <v>64.38515081206496</v>
+        <v>55.4524361948956</v>
       </c>
       <c r="I56" t="n">
-        <v>12.14719577566206</v>
+        <v>12.11146491719338</v>
       </c>
       <c r="J56" t="n">
         <v>29.72413793103448</v>
       </c>
       <c r="K56" t="n">
-        <v>555</v>
+        <v>478</v>
       </c>
       <c r="L56" t="n">
         <v>862</v>
       </c>
       <c r="M56" t="n">
-        <v>3.595127610208817</v>
+        <v>3.160092807424594</v>
       </c>
       <c r="N56" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O56" t="n">
         <v>9.241299303944315</v>
@@ -3342,25 +3342,25 @@
         <v>34.59090909090909</v>
       </c>
       <c r="H57" t="n">
-        <v>69.38239159001314</v>
+        <v>61.36662286465177</v>
       </c>
       <c r="I57" t="n">
-        <v>14.11389320272369</v>
+        <v>14.08183012782224</v>
       </c>
       <c r="J57" t="n">
         <v>34.59090909090909</v>
       </c>
       <c r="K57" t="n">
-        <v>528</v>
+        <v>467</v>
       </c>
       <c r="L57" t="n">
         <v>761</v>
       </c>
       <c r="M57" t="n">
-        <v>3.789750328515112</v>
+        <v>3.390275952693824</v>
       </c>
       <c r="N57" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O57" t="n">
         <v>9.609724047306177</v>
@@ -3393,25 +3393,25 @@
         <v>24.33333333333333</v>
       </c>
       <c r="H58" t="n">
-        <v>64.72602739726028</v>
+        <v>55.82191780821918</v>
       </c>
       <c r="I58" t="n">
-        <v>9.992237442922374</v>
+        <v>9.956621004566209</v>
       </c>
       <c r="J58" t="n">
         <v>24.33333333333333</v>
       </c>
       <c r="K58" t="n">
-        <v>567</v>
+        <v>489</v>
       </c>
       <c r="L58" t="n">
         <v>876</v>
       </c>
       <c r="M58" t="n">
-        <v>3.59703196347032</v>
+        <v>3.146118721461187</v>
       </c>
       <c r="N58" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="O58" t="n">
         <v>9.164383561643836</v>
@@ -3444,25 +3444,25 @@
         <v>23.2972972972973</v>
       </c>
       <c r="H59" t="n">
-        <v>65.42923433874709</v>
+        <v>56.8445475638051</v>
       </c>
       <c r="I59" t="n">
-        <v>9.580635856273908</v>
+        <v>9.546297109174139</v>
       </c>
       <c r="J59" t="n">
         <v>23.2972972972973</v>
       </c>
       <c r="K59" t="n">
-        <v>564</v>
+        <v>490</v>
       </c>
       <c r="L59" t="n">
         <v>862</v>
       </c>
       <c r="M59" t="n">
-        <v>3.650812064965197</v>
+        <v>3.215777262180974</v>
       </c>
       <c r="N59" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="O59" t="n">
         <v>9.21461716937355</v>
@@ -3495,25 +3495,25 @@
         <v>30.52</v>
       </c>
       <c r="H60" t="n">
-        <v>68.93840104849279</v>
+        <v>61.9921363040629</v>
       </c>
       <c r="I60" t="n">
-        <v>12.48375360419397</v>
+        <v>12.45596854521625</v>
       </c>
       <c r="J60" t="n">
         <v>30.52</v>
       </c>
       <c r="K60" t="n">
-        <v>526</v>
+        <v>473</v>
       </c>
       <c r="L60" t="n">
         <v>763</v>
       </c>
       <c r="M60" t="n">
-        <v>3.773263433813892</v>
+        <v>3.403669724770642</v>
       </c>
       <c r="N60" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O60" t="n">
         <v>9.546526867627785</v>
@@ -3546,25 +3546,25 @@
         <v>34.38095238095238</v>
       </c>
       <c r="H61" t="n">
-        <v>69.94459833795014</v>
+        <v>62.74238227146814</v>
       </c>
       <c r="I61" t="n">
-        <v>14.03215934573275</v>
+        <v>14.00335048146682</v>
       </c>
       <c r="J61" t="n">
         <v>34.38095238095238</v>
       </c>
       <c r="K61" t="n">
-        <v>505</v>
+        <v>453</v>
       </c>
       <c r="L61" t="n">
         <v>722</v>
       </c>
       <c r="M61" t="n">
-        <v>3.833795013850415</v>
+        <v>3.457063711911357</v>
       </c>
       <c r="N61" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O61" t="n">
         <v>9.720221606648199</v>
@@ -3597,25 +3597,25 @@
         <v>29.96</v>
       </c>
       <c r="H62" t="n">
-        <v>68.75834445927904</v>
+        <v>61.81575433911883</v>
       </c>
       <c r="I62" t="n">
-        <v>12.25903337783712</v>
+        <v>12.23126301735648</v>
       </c>
       <c r="J62" t="n">
         <v>29.96</v>
       </c>
       <c r="K62" t="n">
-        <v>515</v>
+        <v>463</v>
       </c>
       <c r="L62" t="n">
         <v>749</v>
       </c>
       <c r="M62" t="n">
-        <v>3.795727636849132</v>
+        <v>3.428571428571428</v>
       </c>
       <c r="N62" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O62" t="n">
         <v>9.647530040053404</v>
@@ -3648,25 +3648,25 @@
         <v>32.91304347826087</v>
       </c>
       <c r="H63" t="n">
-        <v>68.56010568031704</v>
+        <v>61.8229854689564</v>
       </c>
       <c r="I63" t="n">
-        <v>13.43945781402562</v>
+        <v>13.41250933318018</v>
       </c>
       <c r="J63" t="n">
         <v>32.91304347826087</v>
       </c>
       <c r="K63" t="n">
-        <v>519</v>
+        <v>468</v>
       </c>
       <c r="L63" t="n">
         <v>757</v>
       </c>
       <c r="M63" t="n">
-        <v>3.784676354029062</v>
+        <v>3.428005284015852</v>
       </c>
       <c r="N63" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O63" t="n">
         <v>9.620871862615587</v>
@@ -3699,25 +3699,25 @@
         <v>34.66666666666666</v>
       </c>
       <c r="H64" t="n">
-        <v>70.46703296703298</v>
+        <v>62.5</v>
       </c>
       <c r="I64" t="n">
-        <v>14.1485347985348</v>
+        <v>14.11666666666667</v>
       </c>
       <c r="J64" t="n">
         <v>34.66666666666666</v>
       </c>
       <c r="K64" t="n">
-        <v>513</v>
+        <v>455</v>
       </c>
       <c r="L64" t="n">
         <v>728</v>
       </c>
       <c r="M64" t="n">
-        <v>3.850274725274725</v>
+        <v>3.442307692307693</v>
       </c>
       <c r="N64" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O64" t="n">
         <v>9.743131868131869</v>
@@ -3750,25 +3750,25 @@
         <v>27.5</v>
       </c>
       <c r="H65" t="n">
-        <v>69.22077922077922</v>
+        <v>62.07792207792208</v>
       </c>
       <c r="I65" t="n">
-        <v>11.27688311688312</v>
+        <v>11.24831168831169</v>
       </c>
       <c r="J65" t="n">
         <v>27.5</v>
       </c>
       <c r="K65" t="n">
-        <v>533</v>
+        <v>478</v>
       </c>
       <c r="L65" t="n">
         <v>770</v>
       </c>
       <c r="M65" t="n">
-        <v>3.774025974025974</v>
+        <v>3.4</v>
       </c>
       <c r="N65" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O65" t="n">
         <v>9.548051948051947</v>
@@ -3801,25 +3801,25 @@
         <v>23.51428571428572</v>
       </c>
       <c r="H66" t="n">
-        <v>67.07168894289185</v>
+        <v>58.93074119076549</v>
       </c>
       <c r="I66" t="n">
-        <v>9.674001041485855</v>
+        <v>9.641437250477349</v>
       </c>
       <c r="J66" t="n">
         <v>23.51428571428572</v>
       </c>
       <c r="K66" t="n">
-        <v>552</v>
+        <v>485</v>
       </c>
       <c r="L66" t="n">
         <v>823</v>
       </c>
       <c r="M66" t="n">
-        <v>3.663426488456865</v>
+        <v>3.266099635479951</v>
       </c>
       <c r="N66" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="O66" t="n">
         <v>9.334143377885784</v>
@@ -3852,25 +3852,25 @@
         <v>23.24324324324324</v>
       </c>
       <c r="H67" t="n">
-        <v>66.74418604651163</v>
+        <v>59.18604651162791</v>
       </c>
       <c r="I67" t="n">
-        <v>9.564274041483344</v>
+        <v>9.53404148334381</v>
       </c>
       <c r="J67" t="n">
         <v>23.24324324324324</v>
       </c>
       <c r="K67" t="n">
-        <v>574</v>
+        <v>509</v>
       </c>
       <c r="L67" t="n">
         <v>860</v>
       </c>
       <c r="M67" t="n">
-        <v>3.638372093023256</v>
+        <v>3.256976744186046</v>
       </c>
       <c r="N67" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="O67" t="n">
         <v>9.309302325581395</v>
@@ -3903,25 +3903,25 @@
         <v>26.875</v>
       </c>
       <c r="H68" t="n">
-        <v>66.74418604651163</v>
+        <v>59.41860465116279</v>
       </c>
       <c r="I68" t="n">
-        <v>11.01697674418605</v>
+        <v>10.98767441860465</v>
       </c>
       <c r="J68" t="n">
         <v>26.875</v>
       </c>
       <c r="K68" t="n">
-        <v>574</v>
+        <v>511</v>
       </c>
       <c r="L68" t="n">
         <v>860</v>
       </c>
       <c r="M68" t="n">
-        <v>3.626744186046511</v>
+        <v>3.25</v>
       </c>
       <c r="N68" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="O68" t="n">
         <v>9.182558139534883</v>
@@ -3954,25 +3954,25 @@
         <v>21.59523809523809</v>
       </c>
       <c r="H69" t="n">
-        <v>61.63175303197354</v>
+        <v>54.35501653803748</v>
       </c>
       <c r="I69" t="n">
-        <v>8.884622250223133</v>
+        <v>8.855515304247389</v>
       </c>
       <c r="J69" t="n">
         <v>21.59523809523809</v>
       </c>
       <c r="K69" t="n">
-        <v>559</v>
+        <v>493</v>
       </c>
       <c r="L69" t="n">
         <v>907</v>
       </c>
       <c r="M69" t="n">
-        <v>3.498346196251378</v>
+        <v>3.138919514884234</v>
       </c>
       <c r="N69" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="O69" t="n">
         <v>8.997794928335171</v>
@@ -4005,25 +4005,25 @@
         <v>24.8</v>
       </c>
       <c r="H70" t="n">
-        <v>69.23963133640552</v>
+        <v>61.9815668202765</v>
       </c>
       <c r="I70" t="n">
-        <v>10.19695852534562</v>
+        <v>10.16792626728111</v>
       </c>
       <c r="J70" t="n">
         <v>24.8</v>
       </c>
       <c r="K70" t="n">
-        <v>601</v>
+        <v>538</v>
       </c>
       <c r="L70" t="n">
         <v>868</v>
       </c>
       <c r="M70" t="n">
-        <v>3.661290322580645</v>
+        <v>3.299539170506912</v>
       </c>
       <c r="N70" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="O70" t="n">
         <v>9.198156682027649</v>
@@ -4056,25 +4056,25 @@
         <v>31.5</v>
       </c>
       <c r="H71" t="n">
-        <v>68.25396825396825</v>
+        <v>60.07326007326007</v>
       </c>
       <c r="I71" t="n">
-        <v>12.87301587301587</v>
+        <v>12.84029304029304</v>
       </c>
       <c r="J71" t="n">
         <v>31.5</v>
       </c>
       <c r="K71" t="n">
-        <v>559</v>
+        <v>492</v>
       </c>
       <c r="L71" t="n">
         <v>819</v>
       </c>
       <c r="M71" t="n">
-        <v>3.705738705738706</v>
+        <v>3.291819291819292</v>
       </c>
       <c r="N71" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="O71" t="n">
         <v>9.411477411477412</v>
@@ -4107,25 +4107,25 @@
         <v>21.7037037037037</v>
       </c>
       <c r="H72" t="n">
-        <v>62.37201365187713</v>
+        <v>53.24232081911263</v>
       </c>
       <c r="I72" t="n">
-        <v>8.930969536088989</v>
+        <v>8.894450764757933</v>
       </c>
       <c r="J72" t="n">
         <v>21.7037037037037</v>
       </c>
       <c r="K72" t="n">
-        <v>731</v>
+        <v>624</v>
       </c>
       <c r="L72" t="n">
         <v>1172</v>
       </c>
       <c r="M72" t="n">
-        <v>3.408703071672355</v>
+        <v>2.984641638225256</v>
       </c>
       <c r="N72" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="O72" t="n">
         <v>8.709044368600683</v>
@@ -4158,25 +4158,25 @@
         <v>28.7741935483871</v>
       </c>
       <c r="H73" t="n">
-        <v>61.54708520179371</v>
+        <v>55.26905829596412</v>
       </c>
       <c r="I73" t="n">
-        <v>11.75586576016201</v>
+        <v>11.7307536525387</v>
       </c>
       <c r="J73" t="n">
         <v>28.7741935483871</v>
       </c>
       <c r="K73" t="n">
-        <v>549</v>
+        <v>493</v>
       </c>
       <c r="L73" t="n">
         <v>892</v>
       </c>
       <c r="M73" t="n">
-        <v>3.513452914798206</v>
+        <v>3.177130044843049</v>
       </c>
       <c r="N73" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="O73" t="n">
         <v>9.050448430493274</v>
@@ -4209,25 +4209,25 @@
         <v>26.625</v>
       </c>
       <c r="H74" t="n">
-        <v>65.72769953051643</v>
+        <v>58.80281690140845</v>
       </c>
       <c r="I74" t="n">
-        <v>10.91291079812207</v>
+        <v>10.88521126760563</v>
       </c>
       <c r="J74" t="n">
         <v>26.625</v>
       </c>
       <c r="K74" t="n">
-        <v>560</v>
+        <v>501</v>
       </c>
       <c r="L74" t="n">
         <v>852</v>
       </c>
       <c r="M74" t="n">
-        <v>3.647887323943662</v>
+        <v>3.269953051643192</v>
       </c>
       <c r="N74" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O74" t="n">
         <v>9.342723004694836</v>
@@ -4260,25 +4260,25 @@
         <v>32.125</v>
       </c>
       <c r="H75" t="n">
-        <v>64.07263294422827</v>
+        <v>57.71725032425421</v>
       </c>
       <c r="I75" t="n">
-        <v>13.10629053177691</v>
+        <v>13.08086900129702</v>
       </c>
       <c r="J75" t="n">
         <v>32.125</v>
       </c>
       <c r="K75" t="n">
-        <v>494</v>
+        <v>445</v>
       </c>
       <c r="L75" t="n">
         <v>771</v>
       </c>
       <c r="M75" t="n">
-        <v>3.675745784695201</v>
+        <v>3.316472114137484</v>
       </c>
       <c r="N75" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O75" t="n">
         <v>9.354085603112841</v>
@@ -4311,25 +4311,25 @@
         <v>27.06451612903226</v>
       </c>
       <c r="H76" t="n">
-        <v>66.15017878426698</v>
+        <v>59.35637663885578</v>
       </c>
       <c r="I76" t="n">
-        <v>11.09040716674997</v>
+        <v>11.06323195816833</v>
       </c>
       <c r="J76" t="n">
         <v>27.06451612903226</v>
       </c>
       <c r="K76" t="n">
-        <v>555</v>
+        <v>498</v>
       </c>
       <c r="L76" t="n">
         <v>839</v>
       </c>
       <c r="M76" t="n">
-        <v>3.64958283671037</v>
+        <v>3.286054827175209</v>
       </c>
       <c r="N76" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="O76" t="n">
         <v>9.34207389749702</v>
@@ -4362,25 +4362,25 @@
         <v>27.125</v>
       </c>
       <c r="H77" t="n">
-        <v>65.32258064516128</v>
+        <v>58.6405529953917</v>
       </c>
       <c r="I77" t="n">
-        <v>11.11129032258065</v>
+        <v>11.08456221198157</v>
       </c>
       <c r="J77" t="n">
         <v>27.125</v>
       </c>
       <c r="K77" t="n">
-        <v>567</v>
+        <v>509</v>
       </c>
       <c r="L77" t="n">
         <v>868</v>
       </c>
       <c r="M77" t="n">
-        <v>3.579493087557604</v>
+        <v>3.223502304147465</v>
       </c>
       <c r="N77" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="O77" t="n">
         <v>9.139400921658986</v>
@@ -4413,25 +4413,25 @@
         <v>30.44444444444444</v>
       </c>
       <c r="H78" t="n">
-        <v>66.54501216545012</v>
+        <v>57.90754257907543</v>
       </c>
       <c r="I78" t="n">
-        <v>12.44395782643958</v>
+        <v>12.40940794809408</v>
       </c>
       <c r="J78" t="n">
         <v>30.44444444444444</v>
       </c>
       <c r="K78" t="n">
-        <v>547</v>
+        <v>476</v>
       </c>
       <c r="L78" t="n">
         <v>822</v>
       </c>
       <c r="M78" t="n">
-        <v>3.665450121654501</v>
+        <v>3.25669099756691</v>
       </c>
       <c r="N78" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="O78" t="n">
         <v>9.318734793187348</v>
@@ -4464,25 +4464,25 @@
         <v>29.59259259259259</v>
       </c>
       <c r="H79" t="n">
-        <v>69.96245306633291</v>
+        <v>62.82853566958698</v>
       </c>
       <c r="I79" t="n">
-        <v>12.11688684930237</v>
+        <v>12.08835117971539</v>
       </c>
       <c r="J79" t="n">
         <v>29.59259259259259</v>
       </c>
       <c r="K79" t="n">
-        <v>559</v>
+        <v>502</v>
       </c>
       <c r="L79" t="n">
         <v>799</v>
       </c>
       <c r="M79" t="n">
-        <v>3.801001251564456</v>
+        <v>3.429286608260325</v>
       </c>
       <c r="N79" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="O79" t="n">
         <v>9.531914893617021</v>
@@ -4515,25 +4515,25 @@
         <v>25.42424242424243</v>
       </c>
       <c r="H80" t="n">
-        <v>65.67342073897497</v>
+        <v>58.87961859356376</v>
       </c>
       <c r="I80" t="n">
-        <v>10.43239065265287</v>
+        <v>10.40521544407123</v>
       </c>
       <c r="J80" t="n">
         <v>25.42424242424243</v>
       </c>
       <c r="K80" t="n">
-        <v>551</v>
+        <v>494</v>
       </c>
       <c r="L80" t="n">
         <v>839</v>
       </c>
       <c r="M80" t="n">
-        <v>3.636471990464839</v>
+        <v>3.280095351609059</v>
       </c>
       <c r="N80" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="O80" t="n">
         <v>9.191895113230036</v>
@@ -4566,25 +4566,25 @@
         <v>26.54285714285714</v>
       </c>
       <c r="H81" t="n">
-        <v>63.07857911733046</v>
+        <v>55.75888051668461</v>
       </c>
       <c r="I81" t="n">
-        <v>10.86945717361218</v>
+        <v>10.8401783792096</v>
       </c>
       <c r="J81" t="n">
         <v>26.54285714285714</v>
       </c>
       <c r="K81" t="n">
-        <v>586</v>
+        <v>518</v>
       </c>
       <c r="L81" t="n">
         <v>929</v>
       </c>
       <c r="M81" t="n">
-        <v>3.470398277717976</v>
+        <v>3.11194833153929</v>
       </c>
       <c r="N81" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O81" t="n">
         <v>9.011840688912809</v>
@@ -4617,25 +4617,25 @@
         <v>25.14705882352941</v>
       </c>
       <c r="H82" t="n">
-        <v>66.43274853801169</v>
+        <v>58.47953216374269</v>
       </c>
       <c r="I82" t="n">
-        <v>10.32455452356381</v>
+        <v>10.29274165806674</v>
       </c>
       <c r="J82" t="n">
         <v>25.14705882352941</v>
       </c>
       <c r="K82" t="n">
-        <v>568</v>
+        <v>500</v>
       </c>
       <c r="L82" t="n">
         <v>855</v>
       </c>
       <c r="M82" t="n">
-        <v>3.632748538011696</v>
+        <v>3.223391812865497</v>
       </c>
       <c r="N82" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O82" t="n">
         <v>9.266666666666667</v>
@@ -4668,25 +4668,25 @@
         <v>38.2</v>
       </c>
       <c r="H83" t="n">
-        <v>66.8848167539267</v>
+        <v>59.55497382198953</v>
       </c>
       <c r="I83" t="n">
-        <v>15.54753926701571</v>
+        <v>15.51821989528796</v>
       </c>
       <c r="J83" t="n">
         <v>38.2</v>
       </c>
       <c r="K83" t="n">
-        <v>511</v>
+        <v>455</v>
       </c>
       <c r="L83" t="n">
         <v>764</v>
       </c>
       <c r="M83" t="n">
-        <v>3.735602094240838</v>
+        <v>3.352094240837696</v>
       </c>
       <c r="N83" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O83" t="n">
         <v>9.518324607329843</v>
@@ -4719,25 +4719,25 @@
         <v>24.63636363636364</v>
       </c>
       <c r="H84" t="n">
-        <v>65.19065190651907</v>
+        <v>58.05658056580566</v>
       </c>
       <c r="I84" t="n">
-        <v>10.11530806217153</v>
+        <v>10.08677177680868</v>
       </c>
       <c r="J84" t="n">
         <v>24.63636363636364</v>
       </c>
       <c r="K84" t="n">
-        <v>530</v>
+        <v>472</v>
       </c>
       <c r="L84" t="n">
         <v>813</v>
       </c>
       <c r="M84" t="n">
-        <v>3.674046740467405</v>
+        <v>3.297662976629766</v>
       </c>
       <c r="N84" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O84" t="n">
         <v>9.392373923739237</v>
@@ -4770,25 +4770,25 @@
         <v>29.78571428571428</v>
       </c>
       <c r="H85" t="n">
-        <v>64.98800959232614</v>
+        <v>57.31414868105516</v>
       </c>
       <c r="I85" t="n">
-        <v>12.17423775265502</v>
+        <v>12.14354230900994</v>
       </c>
       <c r="J85" t="n">
         <v>29.78571428571428</v>
       </c>
       <c r="K85" t="n">
-        <v>542</v>
+        <v>478</v>
       </c>
       <c r="L85" t="n">
         <v>834</v>
       </c>
       <c r="M85" t="n">
-        <v>3.65347721822542</v>
+        <v>3.255395683453238</v>
       </c>
       <c r="N85" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O85" t="n">
         <v>9.311750599520384</v>
@@ -4821,25 +4821,25 @@
         <v>31.84</v>
       </c>
       <c r="H86" t="n">
-        <v>66.08040201005025</v>
+        <v>59.2964824120603</v>
       </c>
       <c r="I86" t="n">
-        <v>13.0003216080402</v>
+        <v>12.97318592964824</v>
       </c>
       <c r="J86" t="n">
         <v>31.84</v>
       </c>
       <c r="K86" t="n">
-        <v>526</v>
+        <v>472</v>
       </c>
       <c r="L86" t="n">
         <v>796</v>
       </c>
       <c r="M86" t="n">
-        <v>3.706030150753769</v>
+        <v>3.335427135678392</v>
       </c>
       <c r="N86" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O86" t="n">
         <v>9.381909547738694</v>
@@ -4872,25 +4872,25 @@
         <v>48.8125</v>
       </c>
       <c r="H87" t="n">
-        <v>66.58130601792574</v>
+        <v>59.53905249679897</v>
       </c>
       <c r="I87" t="n">
-        <v>19.79132522407171</v>
+        <v>19.7631562099872</v>
       </c>
       <c r="J87" t="n">
         <v>48.8125</v>
       </c>
       <c r="K87" t="n">
-        <v>520</v>
+        <v>465</v>
       </c>
       <c r="L87" t="n">
         <v>781</v>
       </c>
       <c r="M87" t="n">
-        <v>3.69270166453265</v>
+        <v>3.314980793854033</v>
       </c>
       <c r="N87" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O87" t="n">
         <v>9.348271446862997</v>
@@ -4923,25 +4923,25 @@
         <v>25.53125</v>
       </c>
       <c r="H88" t="n">
-        <v>66.95226438188494</v>
+        <v>59.97552019583844</v>
       </c>
       <c r="I88" t="n">
-        <v>10.48030905752754</v>
+        <v>10.45240208078335</v>
       </c>
       <c r="J88" t="n">
         <v>25.53125</v>
       </c>
       <c r="K88" t="n">
-        <v>547</v>
+        <v>490</v>
       </c>
       <c r="L88" t="n">
         <v>817</v>
       </c>
       <c r="M88" t="n">
-        <v>3.692778457772338</v>
+        <v>3.30110159118727</v>
       </c>
       <c r="N88" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O88" t="n">
         <v>9.384332925336597</v>
@@ -4974,25 +4974,25 @@
         <v>19.90909090909091</v>
       </c>
       <c r="H89" t="n">
-        <v>64.95433789954338</v>
+        <v>58.10502283105022</v>
       </c>
       <c r="I89" t="n">
-        <v>8.223453715234539</v>
+        <v>8.196056454960566</v>
       </c>
       <c r="J89" t="n">
         <v>19.90909090909091</v>
       </c>
       <c r="K89" t="n">
-        <v>569</v>
+        <v>509</v>
       </c>
       <c r="L89" t="n">
         <v>876</v>
       </c>
       <c r="M89" t="n">
-        <v>3.638127853881278</v>
+        <v>3.263698630136986</v>
       </c>
       <c r="N89" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="O89" t="n">
         <v>9.242009132420092</v>
@@ -5025,25 +5025,25 @@
         <v>19.06521739130435</v>
       </c>
       <c r="H90" t="n">
-        <v>63.16989737742303</v>
+        <v>56.55644241733181</v>
       </c>
       <c r="I90" t="n">
-        <v>7.878766546031432</v>
+        <v>7.852312726191066</v>
       </c>
       <c r="J90" t="n">
         <v>19.06521739130435</v>
       </c>
       <c r="K90" t="n">
-        <v>554</v>
+        <v>496</v>
       </c>
       <c r="L90" t="n">
         <v>877</v>
       </c>
       <c r="M90" t="n">
-        <v>3.565564424173318</v>
+        <v>3.189281641961232</v>
       </c>
       <c r="N90" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O90" t="n">
         <v>9.076396807297606</v>
@@ -5076,25 +5076,25 @@
         <v>47.76470588235294</v>
       </c>
       <c r="H91" t="n">
-        <v>67.24137931034483</v>
+        <v>60.71428571428571</v>
       </c>
       <c r="I91" t="n">
-        <v>19.37484787018256</v>
+        <v>19.34873949579832</v>
       </c>
       <c r="J91" t="n">
         <v>47.76470588235294</v>
       </c>
       <c r="K91" t="n">
-        <v>546</v>
+        <v>493</v>
       </c>
       <c r="L91" t="n">
         <v>812</v>
       </c>
       <c r="M91" t="n">
-        <v>3.661330049261084</v>
+        <v>3.316502463054187</v>
       </c>
       <c r="N91" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O91" t="n">
         <v>9.198275862068966</v>
@@ -5127,25 +5127,25 @@
         <v>41.05</v>
       </c>
       <c r="H92" t="n">
-        <v>65.40803897685748</v>
+        <v>58.7088915956151</v>
       </c>
       <c r="I92" t="n">
-        <v>16.68163215590743</v>
+        <v>16.65483556638246</v>
       </c>
       <c r="J92" t="n">
         <v>41.05</v>
       </c>
       <c r="K92" t="n">
-        <v>537</v>
+        <v>482</v>
       </c>
       <c r="L92" t="n">
         <v>821</v>
       </c>
       <c r="M92" t="n">
-        <v>3.617539585870889</v>
+        <v>3.270401948842875</v>
       </c>
       <c r="N92" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O92" t="n">
         <v>9.261875761266747</v>
@@ -5178,25 +5178,25 @@
         <v>17.83582089552239</v>
       </c>
       <c r="H93" t="n">
-        <v>65.02092050209205</v>
+        <v>58.32635983263599</v>
       </c>
       <c r="I93" t="n">
-        <v>7.394412040217325</v>
+        <v>7.367633797539501</v>
       </c>
       <c r="J93" t="n">
         <v>17.83582089552239</v>
       </c>
       <c r="K93" t="n">
-        <v>777</v>
+        <v>697</v>
       </c>
       <c r="L93" t="n">
         <v>1195</v>
       </c>
       <c r="M93" t="n">
-        <v>3.34560669456067</v>
+        <v>3.00836820083682</v>
       </c>
       <c r="N93" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O93" t="n">
         <v>8.600836820083682</v>
@@ -5229,25 +5229,25 @@
         <v>19.25396825396825</v>
       </c>
       <c r="H94" t="n">
-        <v>63.56141797197032</v>
+        <v>56.63643858202803</v>
       </c>
       <c r="I94" t="n">
-        <v>7.955832973475182</v>
+        <v>7.928133055915414</v>
       </c>
       <c r="J94" t="n">
         <v>19.25396825396825</v>
       </c>
       <c r="K94" t="n">
-        <v>771</v>
+        <v>687</v>
       </c>
       <c r="L94" t="n">
         <v>1213</v>
       </c>
       <c r="M94" t="n">
-        <v>3.348722176422094</v>
+        <v>3.017312448474856</v>
       </c>
       <c r="N94" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O94" t="n">
         <v>8.550700741962077</v>
@@ -5280,25 +5280,25 @@
         <v>28.14285714285714</v>
       </c>
       <c r="H95" t="n">
-        <v>68.1472081218274</v>
+        <v>61.04060913705583</v>
       </c>
       <c r="I95" t="n">
-        <v>11.52973168963017</v>
+        <v>11.50130529369108</v>
       </c>
       <c r="J95" t="n">
         <v>28.14285714285714</v>
       </c>
       <c r="K95" t="n">
-        <v>537</v>
+        <v>481</v>
       </c>
       <c r="L95" t="n">
         <v>788</v>
       </c>
       <c r="M95" t="n">
-        <v>3.739847715736041</v>
+        <v>3.356598984771574</v>
       </c>
       <c r="N95" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O95" t="n">
         <v>9.447969543147208</v>
@@ -5331,25 +5331,25 @@
         <v>23.62857142857143</v>
       </c>
       <c r="H96" t="n">
-        <v>66.0217654171705</v>
+        <v>58.40386940749698</v>
       </c>
       <c r="I96" t="n">
-        <v>9.715515633097255</v>
+        <v>9.685044049058561</v>
       </c>
       <c r="J96" t="n">
         <v>23.62857142857143</v>
       </c>
       <c r="K96" t="n">
-        <v>546</v>
+        <v>483</v>
       </c>
       <c r="L96" t="n">
         <v>827</v>
       </c>
       <c r="M96" t="n">
-        <v>3.638452237001209</v>
+        <v>3.259975816203144</v>
       </c>
       <c r="N96" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O96" t="n">
         <v>9.222490931076178</v>
@@ -5382,25 +5382,25 @@
         <v>28.66666666666667</v>
       </c>
       <c r="H97" t="n">
-        <v>67.31266149870801</v>
+        <v>59.17312661498708</v>
       </c>
       <c r="I97" t="n">
-        <v>11.7359173126615</v>
+        <v>11.70335917312662</v>
       </c>
       <c r="J97" t="n">
         <v>28.66666666666667</v>
       </c>
       <c r="K97" t="n">
-        <v>521</v>
+        <v>458</v>
       </c>
       <c r="L97" t="n">
         <v>774</v>
       </c>
       <c r="M97" t="n">
-        <v>3.739018087855297</v>
+        <v>3.332041343669251</v>
       </c>
       <c r="N97" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O97" t="n">
         <v>9.488372093023257</v>
@@ -5433,25 +5433,25 @@
         <v>24.44117647058824</v>
       </c>
       <c r="H98" t="n">
-        <v>64.38026474127557</v>
+        <v>56.9193742478941</v>
       </c>
       <c r="I98" t="n">
-        <v>10.0339916472004</v>
+        <v>10.00414808522687</v>
       </c>
       <c r="J98" t="n">
         <v>24.44117647058824</v>
       </c>
       <c r="K98" t="n">
-        <v>535</v>
+        <v>473</v>
       </c>
       <c r="L98" t="n">
         <v>831</v>
       </c>
       <c r="M98" t="n">
-        <v>3.641395908543923</v>
+        <v>3.243080625752106</v>
       </c>
       <c r="N98" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O98" t="n">
         <v>9.247894103489772</v>
@@ -5484,25 +5484,25 @@
         <v>29.84615384615385</v>
       </c>
       <c r="H99" t="n">
-        <v>70.10309278350515</v>
+        <v>63.14432989690722</v>
       </c>
       <c r="I99" t="n">
-        <v>12.21887390959556</v>
+        <v>12.19103885804917</v>
       </c>
       <c r="J99" t="n">
         <v>29.84615384615385</v>
       </c>
       <c r="K99" t="n">
-        <v>544</v>
+        <v>490</v>
       </c>
       <c r="L99" t="n">
         <v>776</v>
       </c>
       <c r="M99" t="n">
-        <v>3.791237113402062</v>
+        <v>3.421391752577319</v>
       </c>
       <c r="N99" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O99" t="n">
         <v>9.610824742268042</v>
@@ -5535,25 +5535,25 @@
         <v>30</v>
       </c>
       <c r="H100" t="n">
-        <v>67</v>
+        <v>59.88888888888889</v>
       </c>
       <c r="I100" t="n">
-        <v>12.268</v>
+        <v>12.23955555555556</v>
       </c>
       <c r="J100" t="n">
         <v>30</v>
       </c>
       <c r="K100" t="n">
-        <v>603</v>
+        <v>539</v>
       </c>
       <c r="L100" t="n">
         <v>900</v>
       </c>
       <c r="M100" t="n">
-        <v>3.661111111111111</v>
+        <v>3.277777777777778</v>
       </c>
       <c r="N100" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="O100" t="n">
         <v>9.384444444444444</v>
@@ -5586,25 +5586,25 @@
         <v>24.93548387096774</v>
       </c>
       <c r="H101" t="n">
-        <v>68.04657179818886</v>
+        <v>61.70763260025873</v>
       </c>
       <c r="I101" t="n">
-        <v>10.24637983557985</v>
+        <v>10.22102407878813</v>
       </c>
       <c r="J101" t="n">
         <v>24.93548387096774</v>
       </c>
       <c r="K101" t="n">
-        <v>526</v>
+        <v>477</v>
       </c>
       <c r="L101" t="n">
         <v>773</v>
       </c>
       <c r="M101" t="n">
-        <v>3.763260025873221</v>
+        <v>3.41914618369987</v>
       </c>
       <c r="N101" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="O101" t="n">
         <v>9.479948253557568</v>
@@ -5637,25 +5637,25 @@
         <v>24.75757575757576</v>
       </c>
       <c r="H102" t="n">
-        <v>65.48347613219094</v>
+        <v>58.01713586291309</v>
       </c>
       <c r="I102" t="n">
-        <v>10.16496420755907</v>
+        <v>10.13509884648196</v>
       </c>
       <c r="J102" t="n">
         <v>24.75757575757576</v>
       </c>
       <c r="K102" t="n">
-        <v>535</v>
+        <v>474</v>
       </c>
       <c r="L102" t="n">
         <v>817</v>
       </c>
       <c r="M102" t="n">
-        <v>3.649938800489596</v>
+        <v>3.258261933904529</v>
       </c>
       <c r="N102" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="O102" t="n">
         <v>9.260709914320685</v>
@@ -5688,25 +5688,25 @@
         <v>30.53846153846154</v>
       </c>
       <c r="H103" t="n">
-        <v>67.63224181360201</v>
+        <v>60.45340050377834</v>
       </c>
       <c r="I103" t="n">
-        <v>12.48591358263903</v>
+        <v>12.45719821739973</v>
       </c>
       <c r="J103" t="n">
         <v>30.53846153846154</v>
       </c>
       <c r="K103" t="n">
-        <v>537</v>
+        <v>480</v>
       </c>
       <c r="L103" t="n">
         <v>794</v>
       </c>
       <c r="M103" t="n">
-        <v>3.702770780856423</v>
+        <v>3.331234256926952</v>
       </c>
       <c r="N103" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="O103" t="n">
         <v>9.416876574307304</v>
@@ -5739,25 +5739,25 @@
         <v>26.26470588235294</v>
       </c>
       <c r="H104" t="n">
-        <v>64.72564389697648</v>
+        <v>57.78275475923852</v>
       </c>
       <c r="I104" t="n">
-        <v>10.76478492852908</v>
+        <v>10.73701337197813</v>
       </c>
       <c r="J104" t="n">
         <v>26.26470588235294</v>
       </c>
       <c r="K104" t="n">
-        <v>578</v>
+        <v>516</v>
       </c>
       <c r="L104" t="n">
         <v>893</v>
       </c>
       <c r="M104" t="n">
-        <v>3.601343784994401</v>
+        <v>3.22508398656215</v>
       </c>
       <c r="N104" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="O104" t="n">
         <v>9.132138857782754</v>
@@ -5790,25 +5790,25 @@
         <v>31.95833333333333</v>
       </c>
       <c r="H105" t="n">
-        <v>66.36245110821382</v>
+        <v>59.19165580182529</v>
       </c>
       <c r="I105" t="n">
-        <v>13.04878313776619</v>
+        <v>13.02009995654063</v>
       </c>
       <c r="J105" t="n">
         <v>31.95833333333333</v>
       </c>
       <c r="K105" t="n">
-        <v>509</v>
+        <v>454</v>
       </c>
       <c r="L105" t="n">
         <v>767</v>
       </c>
       <c r="M105" t="n">
-        <v>3.722294654498044</v>
+        <v>3.332464146023468</v>
       </c>
       <c r="N105" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O105" t="n">
         <v>9.455019556714472</v>
@@ -5841,25 +5841,25 @@
         <v>16.44927536231884</v>
       </c>
       <c r="H106" t="n">
-        <v>61.67400881057269</v>
+        <v>52.68722466960353</v>
       </c>
       <c r="I106" t="n">
-        <v>6.826406180169826</v>
+        <v>6.790459043605951</v>
       </c>
       <c r="J106" t="n">
         <v>16.44927536231884</v>
       </c>
       <c r="K106" t="n">
-        <v>700</v>
+        <v>598</v>
       </c>
       <c r="L106" t="n">
         <v>1135</v>
       </c>
       <c r="M106" t="n">
-        <v>3.390308370044053</v>
+        <v>2.970044052863436</v>
       </c>
       <c r="N106" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O106" t="n">
         <v>8.591189427312775</v>
@@ -5892,25 +5892,25 @@
         <v>20.5</v>
       </c>
       <c r="H107" t="n">
-        <v>60.97560975609756</v>
+        <v>53.65853658536586</v>
       </c>
       <c r="I107" t="n">
-        <v>8.44390243902439</v>
+        <v>8.414634146341463</v>
       </c>
       <c r="J107" t="n">
         <v>20.5</v>
       </c>
       <c r="K107" t="n">
-        <v>575</v>
+        <v>506</v>
       </c>
       <c r="L107" t="n">
         <v>943</v>
       </c>
       <c r="M107" t="n">
-        <v>3.423117709437964</v>
+        <v>3.060445387062566</v>
       </c>
       <c r="N107" t="n">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="O107" t="n">
         <v>8.744432661717921</v>
@@ -5943,25 +5943,25 @@
         <v>27.63333333333333</v>
       </c>
       <c r="H108" t="n">
-        <v>65.98311218335344</v>
+        <v>59.71049457177322</v>
       </c>
       <c r="I108" t="n">
-        <v>11.31726578206675</v>
+        <v>11.29217531162043</v>
       </c>
       <c r="J108" t="n">
         <v>27.63333333333333</v>
       </c>
       <c r="K108" t="n">
-        <v>547</v>
+        <v>495</v>
       </c>
       <c r="L108" t="n">
         <v>829</v>
       </c>
       <c r="M108" t="n">
-        <v>3.605548854041013</v>
+        <v>3.265379975874548</v>
       </c>
       <c r="N108" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O108" t="n">
         <v>9.202653799758746</v>
@@ -5994,25 +5994,25 @@
         <v>39.6</v>
       </c>
       <c r="H109" t="n">
-        <v>68.56060606060606</v>
+        <v>61.86868686868687</v>
       </c>
       <c r="I109" t="n">
-        <v>16.11424242424243</v>
+        <v>16.08747474747475</v>
       </c>
       <c r="J109" t="n">
         <v>39.6</v>
       </c>
       <c r="K109" t="n">
-        <v>543</v>
+        <v>490</v>
       </c>
       <c r="L109" t="n">
         <v>792</v>
       </c>
       <c r="M109" t="n">
-        <v>3.70959595959596</v>
+        <v>3.362373737373737</v>
       </c>
       <c r="N109" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O109" t="n">
         <v>9.382575757575758</v>
@@ -6045,25 +6045,25 @@
         <v>23.55882352941176</v>
       </c>
       <c r="H110" t="n">
-        <v>66.541822721598</v>
+        <v>60.42446941323346</v>
       </c>
       <c r="I110" t="n">
-        <v>9.689696702651098</v>
+        <v>9.66522728941764</v>
       </c>
       <c r="J110" t="n">
         <v>23.55882352941176</v>
       </c>
       <c r="K110" t="n">
-        <v>533</v>
+        <v>484</v>
       </c>
       <c r="L110" t="n">
         <v>801</v>
       </c>
       <c r="M110" t="n">
-        <v>3.694132334581773</v>
+        <v>3.355805243445693</v>
       </c>
       <c r="N110" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="O110" t="n">
         <v>9.309612983770288</v>
@@ -6096,25 +6096,25 @@
         <v>31.33333333333333</v>
       </c>
       <c r="H111" t="n">
-        <v>60.21276595744681</v>
+        <v>53.93617021276596</v>
       </c>
       <c r="I111" t="n">
-        <v>12.77418439716312</v>
+        <v>12.7490780141844</v>
       </c>
       <c r="J111" t="n">
         <v>31.33333333333333</v>
       </c>
       <c r="K111" t="n">
-        <v>566</v>
+        <v>507</v>
       </c>
       <c r="L111" t="n">
         <v>940</v>
       </c>
       <c r="M111" t="n">
-        <v>3.45</v>
+        <v>3.117021276595745</v>
       </c>
       <c r="N111" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="O111" t="n">
         <v>8.853191489361702</v>
@@ -6147,25 +6147,25 @@
         <v>27.17647058823529</v>
       </c>
       <c r="H112" t="n">
-        <v>63.31168831168831</v>
+        <v>57.14285714285714</v>
       </c>
       <c r="I112" t="n">
-        <v>11.12383498854087</v>
+        <v>11.09915966386555</v>
       </c>
       <c r="J112" t="n">
         <v>27.17647058823529</v>
       </c>
       <c r="K112" t="n">
-        <v>585</v>
+        <v>528</v>
       </c>
       <c r="L112" t="n">
         <v>924</v>
       </c>
       <c r="M112" t="n">
-        <v>3.511904761904762</v>
+        <v>3.181818181818182</v>
       </c>
       <c r="N112" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="O112" t="n">
         <v>8.944805194805195</v>
@@ -6198,25 +6198,25 @@
         <v>27.46666666666667</v>
       </c>
       <c r="H113" t="n">
-        <v>64.92718446601941</v>
+        <v>58.00970873786407</v>
       </c>
       <c r="I113" t="n">
-        <v>11.24637540453075</v>
+        <v>11.21870550161812</v>
       </c>
       <c r="J113" t="n">
         <v>27.46666666666667</v>
       </c>
       <c r="K113" t="n">
-        <v>535</v>
+        <v>478</v>
       </c>
       <c r="L113" t="n">
         <v>824</v>
       </c>
       <c r="M113" t="n">
-        <v>3.628640776699029</v>
+        <v>3.263349514563107</v>
       </c>
       <c r="N113" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="O113" t="n">
         <v>9.20752427184466</v>
@@ -6249,25 +6249,25 @@
         <v>24.91891891891892</v>
       </c>
       <c r="H114" t="n">
-        <v>61.49674620390455</v>
+        <v>54.88069414316703</v>
       </c>
       <c r="I114" t="n">
-        <v>10.21355455238319</v>
+        <v>10.18709034414024</v>
       </c>
       <c r="J114" t="n">
         <v>24.91891891891892</v>
       </c>
       <c r="K114" t="n">
-        <v>567</v>
+        <v>506</v>
       </c>
       <c r="L114" t="n">
         <v>922</v>
       </c>
       <c r="M114" t="n">
-        <v>3.523861171366594</v>
+        <v>3.170281995661605</v>
       </c>
       <c r="N114" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="O114" t="n">
         <v>8.962039045553146</v>
@@ -6300,25 +6300,25 @@
         <v>26.27586206896552</v>
       </c>
       <c r="H115" t="n">
-        <v>67.97900262467192</v>
+        <v>61.41732283464567</v>
       </c>
       <c r="I115" t="n">
-        <v>10.78226083808489</v>
+        <v>10.75601411892479</v>
       </c>
       <c r="J115" t="n">
         <v>26.27586206896552</v>
       </c>
       <c r="K115" t="n">
-        <v>518</v>
+        <v>468</v>
       </c>
       <c r="L115" t="n">
         <v>762</v>
       </c>
       <c r="M115" t="n">
-        <v>3.733595800524935</v>
+        <v>3.383202099737533</v>
       </c>
       <c r="N115" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="O115" t="n">
         <v>9.450131233595801</v>
@@ -6351,25 +6351,25 @@
         <v>30.89285714285714</v>
       </c>
       <c r="H116" t="n">
-        <v>69.01734104046243</v>
+        <v>62.42774566473989</v>
       </c>
       <c r="I116" t="n">
-        <v>12.63321222130471</v>
+        <v>12.60685383980182</v>
       </c>
       <c r="J116" t="n">
         <v>30.89285714285714</v>
       </c>
       <c r="K116" t="n">
-        <v>597</v>
+        <v>540</v>
       </c>
       <c r="L116" t="n">
         <v>865</v>
       </c>
       <c r="M116" t="n">
-        <v>3.730635838150289</v>
+        <v>3.383815028901734</v>
       </c>
       <c r="N116" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O116" t="n">
         <v>9.448554913294798</v>
@@ -6402,25 +6402,25 @@
         <v>21.15384615384615</v>
       </c>
       <c r="H117" t="n">
-        <v>56.72727272727273</v>
+        <v>49.90909090909091</v>
       </c>
       <c r="I117" t="n">
-        <v>8.688447552447553</v>
+        <v>8.661174825174825</v>
       </c>
       <c r="J117" t="n">
         <v>21.15384615384615</v>
       </c>
       <c r="K117" t="n">
-        <v>624</v>
+        <v>549</v>
       </c>
       <c r="L117" t="n">
         <v>1100</v>
       </c>
       <c r="M117" t="n">
-        <v>3.211818181818182</v>
+        <v>2.873636363636364</v>
       </c>
       <c r="N117" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="O117" t="n">
         <v>8.299090909090909</v>
@@ -6453,25 +6453,25 @@
         <v>20.95774647887324</v>
       </c>
       <c r="H118" t="n">
-        <v>55.98118279569893</v>
+        <v>49.32795698924731</v>
       </c>
       <c r="I118" t="n">
-        <v>8.607023322732092</v>
+        <v>8.580410419506284</v>
       </c>
       <c r="J118" t="n">
         <v>20.95774647887324</v>
       </c>
       <c r="K118" t="n">
-        <v>833</v>
+        <v>734</v>
       </c>
       <c r="L118" t="n">
         <v>1488</v>
       </c>
       <c r="M118" t="n">
-        <v>3.11760752688172</v>
+        <v>2.782930107526882</v>
       </c>
       <c r="N118" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="O118" t="n">
         <v>7.913306451612903</v>
@@ -6504,25 +6504,25 @@
         <v>27.36585365853659</v>
       </c>
       <c r="H119" t="n">
-        <v>58.28877005347594</v>
+        <v>50.89126559714795</v>
       </c>
       <c r="I119" t="n">
-        <v>11.17949654362854</v>
+        <v>11.14990652580323</v>
       </c>
       <c r="J119" t="n">
         <v>27.36585365853659</v>
       </c>
       <c r="K119" t="n">
-        <v>654</v>
+        <v>571</v>
       </c>
       <c r="L119" t="n">
         <v>1122</v>
       </c>
       <c r="M119" t="n">
-        <v>3.322638146167558</v>
+        <v>2.961675579322638</v>
       </c>
       <c r="N119" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="O119" t="n">
         <v>8.470588235294118</v>
@@ -6555,25 +6555,25 @@
         <v>17.23255813953488</v>
       </c>
       <c r="H120" t="n">
-        <v>67.47638326585695</v>
+        <v>60.72874493927125</v>
       </c>
       <c r="I120" t="n">
-        <v>7.162928788877382</v>
+        <v>7.135938235571039</v>
       </c>
       <c r="J120" t="n">
         <v>17.23255813953488</v>
       </c>
       <c r="K120" t="n">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="L120" t="n">
         <v>741</v>
       </c>
       <c r="M120" t="n">
-        <v>3.709851551956815</v>
+        <v>3.348178137651822</v>
       </c>
       <c r="N120" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O120" t="n">
         <v>9.421052631578947</v>
@@ -6606,25 +6606,25 @@
         <v>32.1304347826087</v>
       </c>
       <c r="H121" t="n">
-        <v>70.77131258457375</v>
+        <v>64.27604871447903</v>
       </c>
       <c r="I121" t="n">
-        <v>13.13525916338177</v>
+        <v>13.1092781079014</v>
       </c>
       <c r="J121" t="n">
         <v>32.1304347826087</v>
       </c>
       <c r="K121" t="n">
-        <v>523</v>
+        <v>475</v>
       </c>
       <c r="L121" t="n">
         <v>739</v>
       </c>
       <c r="M121" t="n">
-        <v>3.822733423545332</v>
+        <v>3.468200270635994</v>
       </c>
       <c r="N121" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O121" t="n">
         <v>9.645466847090663</v>
@@ -6657,25 +6657,25 @@
         <v>31.26086956521739</v>
       </c>
       <c r="H122" t="n">
-        <v>69.12378303198888</v>
+        <v>62.58692628650904</v>
       </c>
       <c r="I122" t="n">
-        <v>12.78084295821491</v>
+        <v>12.75469553123299</v>
       </c>
       <c r="J122" t="n">
         <v>31.26086956521739</v>
       </c>
       <c r="K122" t="n">
-        <v>497</v>
+        <v>450</v>
       </c>
       <c r="L122" t="n">
         <v>719</v>
       </c>
       <c r="M122" t="n">
-        <v>3.833101529902643</v>
+        <v>3.47009735744089</v>
       </c>
       <c r="N122" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O122" t="n">
         <v>9.709318497913769</v>
@@ -6708,25 +6708,25 @@
         <v>37.05</v>
       </c>
       <c r="H123" t="n">
-        <v>67.47638326585695</v>
+        <v>61.1336032388664</v>
       </c>
       <c r="I123" t="n">
-        <v>15.08990553306343</v>
+        <v>15.06453441295547</v>
       </c>
       <c r="J123" t="n">
         <v>37.05</v>
       </c>
       <c r="K123" t="n">
-        <v>500</v>
+        <v>453</v>
       </c>
       <c r="L123" t="n">
         <v>741</v>
       </c>
       <c r="M123" t="n">
-        <v>3.777327935222672</v>
+        <v>3.41970310391363</v>
       </c>
       <c r="N123" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O123" t="n">
         <v>9.587044534412955</v>
@@ -6759,25 +6759,25 @@
         <v>31.04347826086957</v>
       </c>
       <c r="H124" t="n">
-        <v>70.86834733893558</v>
+        <v>64.00560224089635</v>
       </c>
       <c r="I124" t="n">
-        <v>12.70086469370357</v>
+        <v>12.67341371331141</v>
       </c>
       <c r="J124" t="n">
         <v>31.04347826086957</v>
       </c>
       <c r="K124" t="n">
-        <v>506</v>
+        <v>457</v>
       </c>
       <c r="L124" t="n">
         <v>714</v>
       </c>
       <c r="M124" t="n">
-        <v>3.854341736694678</v>
+        <v>3.483193277310924</v>
       </c>
       <c r="N124" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O124" t="n">
         <v>9.733893557422968</v>
@@ -6810,25 +6810,25 @@
         <v>32.68181818181818</v>
       </c>
       <c r="H125" t="n">
-        <v>70.79276773296245</v>
+        <v>64.11682892906815</v>
       </c>
       <c r="I125" t="n">
-        <v>13.35589834365912</v>
+        <v>13.32919458844355</v>
       </c>
       <c r="J125" t="n">
         <v>32.68181818181818</v>
       </c>
       <c r="K125" t="n">
-        <v>509</v>
+        <v>461</v>
       </c>
       <c r="L125" t="n">
         <v>719</v>
       </c>
       <c r="M125" t="n">
-        <v>3.835883171070932</v>
+        <v>3.471488178025035</v>
       </c>
       <c r="N125" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O125" t="n">
         <v>9.695410292072323</v>
@@ -6861,25 +6861,25 @@
         <v>21.04166666666667</v>
       </c>
       <c r="H126" t="n">
-        <v>62.17821782178218</v>
+        <v>54.75247524752476</v>
       </c>
       <c r="I126" t="n">
-        <v>8.665379537953795</v>
+        <v>8.635676567656766</v>
       </c>
       <c r="J126" t="n">
         <v>21.04166666666667</v>
       </c>
       <c r="K126" t="n">
-        <v>628</v>
+        <v>553</v>
       </c>
       <c r="L126" t="n">
         <v>1010</v>
       </c>
       <c r="M126" t="n">
-        <v>3.443564356435644</v>
+        <v>3.073267326732673</v>
       </c>
       <c r="N126" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="O126" t="n">
         <v>8.846534653465346</v>
@@ -6912,25 +6912,25 @@
         <v>27</v>
       </c>
       <c r="H127" t="n">
-        <v>68.65079365079364</v>
+        <v>61.11111111111111</v>
       </c>
       <c r="I127" t="n">
-        <v>11.07460317460318</v>
+        <v>11.04444444444444</v>
       </c>
       <c r="J127" t="n">
         <v>27</v>
       </c>
       <c r="K127" t="n">
-        <v>519</v>
+        <v>462</v>
       </c>
       <c r="L127" t="n">
         <v>756</v>
       </c>
       <c r="M127" t="n">
-        <v>3.767195767195767</v>
+        <v>3.374338624338624</v>
       </c>
       <c r="N127" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O127" t="n">
         <v>9.5</v>
@@ -6963,25 +6963,25 @@
         <v>28.9375</v>
       </c>
       <c r="H128" t="n">
-        <v>66.09071274298056</v>
+        <v>57.77537796976242</v>
       </c>
       <c r="I128" t="n">
-        <v>11.83936285097192</v>
+        <v>11.80610151187905</v>
       </c>
       <c r="J128" t="n">
         <v>28.9375</v>
       </c>
       <c r="K128" t="n">
-        <v>612</v>
+        <v>535</v>
       </c>
       <c r="L128" t="n">
         <v>926</v>
       </c>
       <c r="M128" t="n">
-        <v>3.598272138228942</v>
+        <v>3.192224622030237</v>
       </c>
       <c r="N128" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O128" t="n">
         <v>9.056155507559396</v>
@@ -7014,25 +7014,25 @@
         <v>32.29166666666666</v>
       </c>
       <c r="H129" t="n">
-        <v>67.2258064516129</v>
+        <v>60.38709677419355</v>
       </c>
       <c r="I129" t="n">
-        <v>13.18556989247312</v>
+        <v>13.15821505376344</v>
       </c>
       <c r="J129" t="n">
         <v>32.29166666666666</v>
       </c>
       <c r="K129" t="n">
-        <v>521</v>
+        <v>468</v>
       </c>
       <c r="L129" t="n">
         <v>775</v>
       </c>
       <c r="M129" t="n">
-        <v>3.756129032258065</v>
+        <v>3.381935483870968</v>
       </c>
       <c r="N129" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O129" t="n">
         <v>9.530322580645162</v>
@@ -7065,25 +7065,25 @@
         <v>23.55555555555556</v>
       </c>
       <c r="H130" t="n">
-        <v>68.51415094339622</v>
+        <v>60.25943396226415</v>
       </c>
       <c r="I130" t="n">
-        <v>9.696278825995808</v>
+        <v>9.663259958071279</v>
       </c>
       <c r="J130" t="n">
         <v>23.55555555555556</v>
       </c>
       <c r="K130" t="n">
-        <v>581</v>
+        <v>511</v>
       </c>
       <c r="L130" t="n">
         <v>848</v>
       </c>
       <c r="M130" t="n">
-        <v>3.726415094339623</v>
+        <v>3.316037735849056</v>
       </c>
       <c r="N130" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="O130" t="n">
         <v>9.40683962264151</v>
@@ -7116,25 +7116,25 @@
         <v>24.74285714285714</v>
       </c>
       <c r="H131" t="n">
-        <v>63.39491916859122</v>
+        <v>56.9284064665127</v>
       </c>
       <c r="I131" t="n">
-        <v>10.15072253381722</v>
+        <v>10.12485648300891</v>
       </c>
       <c r="J131" t="n">
         <v>24.74285714285714</v>
       </c>
       <c r="K131" t="n">
-        <v>549</v>
+        <v>493</v>
       </c>
       <c r="L131" t="n">
         <v>866</v>
       </c>
       <c r="M131" t="n">
-        <v>3.584295612009238</v>
+        <v>3.233256351039261</v>
       </c>
       <c r="N131" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="O131" t="n">
         <v>9.197459584295611</v>
@@ -7167,25 +7167,25 @@
         <v>24.11428571428571</v>
       </c>
       <c r="H132" t="n">
-        <v>65.28436018957346</v>
+        <v>58.29383886255924</v>
       </c>
       <c r="I132" t="n">
-        <v>9.906851726472581</v>
+        <v>9.878889641164523</v>
       </c>
       <c r="J132" t="n">
         <v>24.11428571428571</v>
       </c>
       <c r="K132" t="n">
-        <v>551</v>
+        <v>492</v>
       </c>
       <c r="L132" t="n">
         <v>844</v>
       </c>
       <c r="M132" t="n">
-        <v>3.626777251184834</v>
+        <v>3.247630331753554</v>
       </c>
       <c r="N132" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O132" t="n">
         <v>9.266587677725118</v>
@@ -7218,25 +7218,25 @@
         <v>26.12903225806452</v>
       </c>
       <c r="H133" t="n">
-        <v>66.91358024691358</v>
+        <v>60.61728395061728</v>
       </c>
       <c r="I133" t="n">
-        <v>10.71926722421346</v>
+        <v>10.69408203902828</v>
       </c>
       <c r="J133" t="n">
         <v>26.12903225806452</v>
       </c>
       <c r="K133" t="n">
-        <v>542</v>
+        <v>491</v>
       </c>
       <c r="L133" t="n">
         <v>810</v>
       </c>
       <c r="M133" t="n">
-        <v>3.68395061728395</v>
+        <v>3.330864197530864</v>
       </c>
       <c r="N133" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="O133" t="n">
         <v>9.388888888888889</v>
@@ -7269,25 +7269,25 @@
         <v>31.76</v>
       </c>
       <c r="H134" t="n">
-        <v>68.01007556675063</v>
+        <v>60.70528967254408</v>
       </c>
       <c r="I134" t="n">
-        <v>12.976040302267</v>
+        <v>12.94682115869018</v>
       </c>
       <c r="J134" t="n">
         <v>31.76</v>
       </c>
       <c r="K134" t="n">
-        <v>540</v>
+        <v>482</v>
       </c>
       <c r="L134" t="n">
         <v>794</v>
       </c>
       <c r="M134" t="n">
-        <v>3.739294710327456</v>
+        <v>3.348866498740554</v>
       </c>
       <c r="N134" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O134" t="n">
         <v>9.385390428211586</v>
@@ -7320,25 +7320,25 @@
         <v>29.55555555555556</v>
       </c>
       <c r="H135" t="n">
-        <v>67.04260651629073</v>
+        <v>58.89724310776943</v>
       </c>
       <c r="I135" t="n">
-        <v>12.09039264828739</v>
+        <v>12.0578111946533</v>
       </c>
       <c r="J135" t="n">
         <v>29.55555555555556</v>
       </c>
       <c r="K135" t="n">
-        <v>535</v>
+        <v>470</v>
       </c>
       <c r="L135" t="n">
         <v>798</v>
       </c>
       <c r="M135" t="n">
-        <v>3.725563909774436</v>
+        <v>3.31203007518797</v>
       </c>
       <c r="N135" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O135" t="n">
         <v>9.414786967418546</v>
@@ -7371,25 +7371,25 @@
         <v>32.25</v>
       </c>
       <c r="H136" t="n">
-        <v>68.34625322997417</v>
+        <v>61.24031007751937</v>
       </c>
       <c r="I136" t="n">
-        <v>13.1733850129199</v>
+        <v>13.14496124031008</v>
       </c>
       <c r="J136" t="n">
         <v>32.25</v>
       </c>
       <c r="K136" t="n">
-        <v>529</v>
+        <v>474</v>
       </c>
       <c r="L136" t="n">
         <v>774</v>
       </c>
       <c r="M136" t="n">
-        <v>3.760981912144703</v>
+        <v>3.386304909560724</v>
       </c>
       <c r="N136" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O136" t="n">
         <v>9.490956072351421</v>
@@ -7422,25 +7422,25 @@
         <v>34.90909090909091</v>
       </c>
       <c r="H137" t="n">
-        <v>68.48958333333334</v>
+        <v>61.328125</v>
       </c>
       <c r="I137" t="n">
-        <v>14.2375946969697</v>
+        <v>14.20894886363636</v>
       </c>
       <c r="J137" t="n">
         <v>34.90909090909091</v>
       </c>
       <c r="K137" t="n">
-        <v>526</v>
+        <v>471</v>
       </c>
       <c r="L137" t="n">
         <v>768</v>
       </c>
       <c r="M137" t="n">
-        <v>3.774739583333333</v>
+        <v>3.399739583333333</v>
       </c>
       <c r="N137" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O137" t="n">
         <v>9.5234375</v>
@@ -7473,25 +7473,25 @@
         <v>23.81818181818182</v>
       </c>
       <c r="H138" t="n">
-        <v>67.43002544529261</v>
+        <v>59.92366412213741</v>
       </c>
       <c r="I138" t="n">
-        <v>9.796992829053899</v>
+        <v>9.766967383761276</v>
       </c>
       <c r="J138" t="n">
         <v>23.81818181818182</v>
       </c>
       <c r="K138" t="n">
-        <v>530</v>
+        <v>471</v>
       </c>
       <c r="L138" t="n">
         <v>786</v>
       </c>
       <c r="M138" t="n">
-        <v>3.723918575063613</v>
+        <v>3.334605597964376</v>
       </c>
       <c r="N138" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O138" t="n">
         <v>9.421119592875318</v>
@@ -7524,25 +7524,25 @@
         <v>33.04166666666666</v>
       </c>
       <c r="H139" t="n">
-        <v>66.33039092055486</v>
+        <v>59.01639344262295</v>
       </c>
       <c r="I139" t="n">
-        <v>13.48198823034888</v>
+        <v>13.45273224043716</v>
       </c>
       <c r="J139" t="n">
         <v>33.04166666666666</v>
       </c>
       <c r="K139" t="n">
-        <v>526</v>
+        <v>468</v>
       </c>
       <c r="L139" t="n">
         <v>793</v>
       </c>
       <c r="M139" t="n">
-        <v>3.697351828499369</v>
+        <v>3.317780580075662</v>
       </c>
       <c r="N139" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O139" t="n">
         <v>9.336696090794451</v>
@@ -7575,25 +7575,25 @@
         <v>30.80769230769231</v>
       </c>
       <c r="H140" t="n">
-        <v>67.16604244694132</v>
+        <v>59.67540574282148</v>
       </c>
       <c r="I140" t="n">
-        <v>12.59174109286469</v>
+        <v>12.56177854604821</v>
       </c>
       <c r="J140" t="n">
         <v>30.80769230769231</v>
       </c>
       <c r="K140" t="n">
-        <v>538</v>
+        <v>478</v>
       </c>
       <c r="L140" t="n">
         <v>801</v>
       </c>
       <c r="M140" t="n">
-        <v>3.701622971285893</v>
+        <v>3.31585518102372</v>
       </c>
       <c r="N140" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O140" t="n">
         <v>9.3083645443196</v>
@@ -7626,25 +7626,25 @@
         <v>23.94444444444444</v>
       </c>
       <c r="H141" t="n">
-        <v>64.15313225058004</v>
+        <v>56.96055684454756</v>
       </c>
       <c r="I141" t="n">
-        <v>9.834390306780099</v>
+        <v>9.805620005155967</v>
       </c>
       <c r="J141" t="n">
         <v>23.94444444444444</v>
       </c>
       <c r="K141" t="n">
-        <v>553</v>
+        <v>491</v>
       </c>
       <c r="L141" t="n">
         <v>862</v>
       </c>
       <c r="M141" t="n">
-        <v>3.603248259860789</v>
+        <v>3.205336426914153</v>
       </c>
       <c r="N141" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O141" t="n">
         <v>9.209976798143851</v>
@@ -7677,25 +7677,25 @@
         <v>16.98550724637681</v>
       </c>
       <c r="H142" t="n">
-        <v>56.0580204778157</v>
+        <v>47.52559726962458</v>
       </c>
       <c r="I142" t="n">
-        <v>7.018434980461987</v>
+        <v>6.984305287629224</v>
       </c>
       <c r="J142" t="n">
         <v>16.98550724637681</v>
       </c>
       <c r="K142" t="n">
-        <v>657</v>
+        <v>557</v>
       </c>
       <c r="L142" t="n">
         <v>1172</v>
       </c>
       <c r="M142" t="n">
-        <v>3.28839590443686</v>
+        <v>2.843856655290102</v>
       </c>
       <c r="N142" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="O142" t="n">
         <v>8.529863481228668</v>
@@ -7728,25 +7728,25 @@
         <v>23.35714285714286</v>
       </c>
       <c r="H143" t="n">
-        <v>67.48216106014272</v>
+        <v>60.55045871559633</v>
       </c>
       <c r="I143" t="n">
-        <v>9.612785787097714</v>
+        <v>9.585058977719529</v>
       </c>
       <c r="J143" t="n">
         <v>23.35714285714286</v>
       </c>
       <c r="K143" t="n">
-        <v>662</v>
+        <v>594</v>
       </c>
       <c r="L143" t="n">
         <v>981</v>
       </c>
       <c r="M143" t="n">
-        <v>3.577981651376147</v>
+        <v>3.221202854230377</v>
       </c>
       <c r="N143" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="O143" t="n">
         <v>9.132517838939858</v>
@@ -7779,25 +7779,25 @@
         <v>21.10909090909091</v>
       </c>
       <c r="H144" t="n">
-        <v>60.98191214470285</v>
+        <v>52.36864771748493</v>
       </c>
       <c r="I144" t="n">
-        <v>8.687564012215175</v>
+        <v>8.653110954506303</v>
       </c>
       <c r="J144" t="n">
         <v>21.10909090909091</v>
       </c>
       <c r="K144" t="n">
-        <v>708</v>
+        <v>608</v>
       </c>
       <c r="L144" t="n">
         <v>1161</v>
       </c>
       <c r="M144" t="n">
-        <v>3.383290267011197</v>
+        <v>2.964685615848407</v>
       </c>
       <c r="N144" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O144" t="n">
         <v>8.648578811369509</v>
@@ -7830,25 +7830,25 @@
         <v>17.54878048780488</v>
       </c>
       <c r="H145" t="n">
-        <v>60.18068102849201</v>
+        <v>52.18902015288395</v>
       </c>
       <c r="I145" t="n">
-        <v>7.260234919235919</v>
+        <v>7.228268275733488</v>
       </c>
       <c r="J145" t="n">
         <v>17.54878048780488</v>
       </c>
       <c r="K145" t="n">
-        <v>866</v>
+        <v>751</v>
       </c>
       <c r="L145" t="n">
         <v>1439</v>
       </c>
       <c r="M145" t="n">
-        <v>3.264767199444059</v>
+        <v>2.887421820708826</v>
       </c>
       <c r="N145" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="O145" t="n">
         <v>8.229325920778319</v>
@@ -7881,25 +7881,25 @@
         <v>21.74358974358974</v>
       </c>
       <c r="H146" t="n">
-        <v>64.97641509433963</v>
+        <v>57.78301886792453</v>
       </c>
       <c r="I146" t="n">
-        <v>8.957341557813256</v>
+        <v>8.928567972907597</v>
       </c>
       <c r="J146" t="n">
         <v>21.74358974358974</v>
       </c>
       <c r="K146" t="n">
-        <v>551</v>
+        <v>490</v>
       </c>
       <c r="L146" t="n">
         <v>848</v>
       </c>
       <c r="M146" t="n">
-        <v>3.613207547169811</v>
+        <v>3.237028301886792</v>
       </c>
       <c r="N146" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="O146" t="n">
         <v>9.163915094339623</v>
@@ -7932,25 +7932,25 @@
         <v>48.46666666666667</v>
       </c>
       <c r="H147" t="n">
-        <v>68.22558459422284</v>
+        <v>60.52269601100413</v>
       </c>
       <c r="I147" t="n">
-        <v>19.65956900504356</v>
+        <v>19.62875745071069</v>
       </c>
       <c r="J147" t="n">
         <v>48.46666666666667</v>
       </c>
       <c r="K147" t="n">
-        <v>496</v>
+        <v>440</v>
       </c>
       <c r="L147" t="n">
         <v>727</v>
       </c>
       <c r="M147" t="n">
-        <v>3.81292984869326</v>
+        <v>3.41678129298487</v>
       </c>
       <c r="N147" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O147" t="n">
         <v>9.675378266850069</v>
@@ -7983,25 +7983,25 @@
         <v>34.09523809523809</v>
       </c>
       <c r="H148" t="n">
-        <v>69.1340782122905</v>
+        <v>62.43016759776536</v>
       </c>
       <c r="I148" t="n">
-        <v>13.9146315509444</v>
+        <v>13.8878159084863</v>
       </c>
       <c r="J148" t="n">
         <v>34.09523809523809</v>
       </c>
       <c r="K148" t="n">
-        <v>495</v>
+        <v>447</v>
       </c>
       <c r="L148" t="n">
         <v>716</v>
       </c>
       <c r="M148" t="n">
-        <v>3.835195530726257</v>
+        <v>3.472067039106145</v>
       </c>
       <c r="N148" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O148" t="n">
         <v>9.69413407821229</v>

</xml_diff>